<commit_message>
add type & comment in table assets
</commit_message>
<xml_diff>
--- a/prisma/seed/seed_data.xlsx
+++ b/prisma/seed/seed_data.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/rafly/Data/Dev/Project/monitoring-welding-body/prisma/seed/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EE8FF63D-7E3C-C241-878F-486D64317714}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2B68DE60-A089-BE43-A7B3-BE0D305782AF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="500" windowWidth="33600" windowHeight="19100" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="722" uniqueCount="686">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1046" uniqueCount="811">
   <si>
     <t>name</t>
   </si>
@@ -2082,6 +2082,381 @@
   </si>
   <si>
     <t>PART161</t>
+  </si>
+  <si>
+    <t>type</t>
+  </si>
+  <si>
+    <t>comment</t>
+  </si>
+  <si>
+    <t>E-CAT COMM. NORMAL</t>
+  </si>
+  <si>
+    <t>DATA PL ID SP1_STOP</t>
+  </si>
+  <si>
+    <t>DATA PL ID SP2 STOP</t>
+  </si>
+  <si>
+    <t>DATA PL ID SP3 STOP</t>
+  </si>
+  <si>
+    <t>DATA PL ID SP4 STOP</t>
+  </si>
+  <si>
+    <t>DATA PL ID SP6 STOP</t>
+  </si>
+  <si>
+    <t>DATA PL ID SP7 STOP</t>
+  </si>
+  <si>
+    <t>DATA PL ID SP8 STOP</t>
+  </si>
+  <si>
+    <t>DATA PL ID SP10 STOP</t>
+  </si>
+  <si>
+    <t>DATA PL ID SP0 STOP</t>
+  </si>
+  <si>
+    <t>EIP OHC 1 FAULT</t>
+  </si>
+  <si>
+    <t>SET INPUT HMI_HIGH SPEED LIFTER</t>
+  </si>
+  <si>
+    <t>SET INPUT HMI_MEDIUM SPEED LIFTER</t>
+  </si>
+  <si>
+    <t>SET INPUT HMI_LOW SPEED LIFTER</t>
+  </si>
+  <si>
+    <t>EIP COMMUNCIATION FAULT_FLG HMI</t>
+  </si>
+  <si>
+    <t>PB DOLLY SET COMPLETE</t>
+  </si>
+  <si>
+    <t>SS4 (MOTRAIN DOWN)</t>
+  </si>
+  <si>
+    <t>SS4 (MOTRAIN UP)</t>
+  </si>
+  <si>
+    <t>SS5 (HANGER ARM OPEN)</t>
+  </si>
+  <si>
+    <t>SS5 (HANGER ARM CLOSE)</t>
+  </si>
+  <si>
+    <t>PB WORK FINISH</t>
+  </si>
+  <si>
+    <t>UNLOADING DOLLY LOCK OK</t>
+  </si>
+  <si>
+    <t>UNLOADING DOLLY OUT COMPLETE</t>
+  </si>
+  <si>
+    <t>BOOL</t>
+  </si>
+  <si>
+    <t>INT</t>
+  </si>
+  <si>
+    <t>REAL</t>
+  </si>
+  <si>
+    <t>ST1 OPEN END</t>
+  </si>
+  <si>
+    <t>ST1 CLOSE END</t>
+  </si>
+  <si>
+    <t>PS1 FOR END</t>
+  </si>
+  <si>
+    <t>PS1 REV END</t>
+  </si>
+  <si>
+    <t>MOTRAIN PRESENT</t>
+  </si>
+  <si>
+    <t>MOTRAIN CLEAR 1</t>
+  </si>
+  <si>
+    <t>MOTRAIN CLEAR 2</t>
+  </si>
+  <si>
+    <t>LOAD DWN END 1</t>
+  </si>
+  <si>
+    <t>LOAD DWN END 2</t>
+  </si>
+  <si>
+    <t>LOAD BODY DETECT</t>
+  </si>
+  <si>
+    <t>ST2 OPEN END</t>
+  </si>
+  <si>
+    <t>ST2 CLOSE END</t>
+  </si>
+  <si>
+    <t>PS2 FOR END</t>
+  </si>
+  <si>
+    <t>PS2 REV END</t>
+  </si>
+  <si>
+    <t>UNLOAD BODY DETECT</t>
+  </si>
+  <si>
+    <t>UNLOAD FL BODY DETECT 1</t>
+  </si>
+  <si>
+    <t>UNLOAD FL BODY DETECT 2</t>
+  </si>
+  <si>
+    <t>SW1-MAIN</t>
+  </si>
+  <si>
+    <t>SW1-REPAIR</t>
+  </si>
+  <si>
+    <t>SP5 DECEL</t>
+  </si>
+  <si>
+    <t>BODY DOLLY IN</t>
+  </si>
+  <si>
+    <t>BODY NG OUT</t>
+  </si>
+  <si>
+    <t>SKID READY</t>
+  </si>
+  <si>
+    <t>SKID OUT</t>
+  </si>
+  <si>
+    <t>BODY READY</t>
+  </si>
+  <si>
+    <t>UNLOADING ALARM 1</t>
+  </si>
+  <si>
+    <t>STOPPER-3 OPEN END</t>
+  </si>
+  <si>
+    <t>STOPPER-3 CLOSE END</t>
+  </si>
+  <si>
+    <t>POSITIONER-3 FORWARD END</t>
+  </si>
+  <si>
+    <t>POSITIONER-3 REVERSE END</t>
+  </si>
+  <si>
+    <t>MOTRAIN PRESENT ST6 (SP8 RFID)</t>
+  </si>
+  <si>
+    <t>MOTRAIN CLEAR 1 ST6 (SP8 RFID)</t>
+  </si>
+  <si>
+    <t>MOTRAIN CLEAR 2 ST6 (SP8 RFID)</t>
+  </si>
+  <si>
+    <t>UNLOADING DOWN END 1</t>
+  </si>
+  <si>
+    <t>UNLOADING DOWN END 2</t>
+  </si>
+  <si>
+    <t>BODY DETECT AT SP8</t>
+  </si>
+  <si>
+    <t>LS TIMING KANBAN DETECT AT LOADING</t>
+  </si>
+  <si>
+    <t>KANBAN DETECT AT LOADING POS</t>
+  </si>
+  <si>
+    <t>LOA LIG ON STABIL</t>
+  </si>
+  <si>
+    <t>UNLOADING DATA NORMAL SIGN</t>
+  </si>
+  <si>
+    <t>CB-C6 POS ST8 OPEN PL</t>
+  </si>
+  <si>
+    <t>CB-C6 POS ST8 CLOSE PL</t>
+  </si>
+  <si>
+    <t>CB-C6 POS ST8 FWD PL</t>
+  </si>
+  <si>
+    <t>CB-C6 POS ST8 RVS PL</t>
+  </si>
+  <si>
+    <t>6_SP1 STOP_1401</t>
+  </si>
+  <si>
+    <t>6_SP2 STOP_1402</t>
+  </si>
+  <si>
+    <t>6_SP3 STOP_1403</t>
+  </si>
+  <si>
+    <t>6_SP4 STOP_1404</t>
+  </si>
+  <si>
+    <t>6_SP5 STOP_1405</t>
+  </si>
+  <si>
+    <t>6_SP6 STOP_1406</t>
+  </si>
+  <si>
+    <t>6_SP7 STOP_1407</t>
+  </si>
+  <si>
+    <t>6_SP8 STOP_1408</t>
+  </si>
+  <si>
+    <t>6_SP9 STOP_ 1409</t>
+  </si>
+  <si>
+    <t>6_SP10 STOP_1410</t>
+  </si>
+  <si>
+    <t>6_SP11 STOP_1411</t>
+  </si>
+  <si>
+    <t>6_SP0 STOP_1420</t>
+  </si>
+  <si>
+    <t>EIP COMM FAULT</t>
+  </si>
+  <si>
+    <t>E-CAT COMM FAULT</t>
+  </si>
+  <si>
+    <t>EMG STOP NORMAL CPC</t>
+  </si>
+  <si>
+    <t>EMG STOP NORMAL MAIN PANEL CPC NORMAL</t>
+  </si>
+  <si>
+    <t>1_SP1 STOP_1401</t>
+  </si>
+  <si>
+    <t>1_SP2 STOP_1402</t>
+  </si>
+  <si>
+    <t>1_SP3 STOP_1403</t>
+  </si>
+  <si>
+    <t>1_SP4 STOP_1404</t>
+  </si>
+  <si>
+    <t>1_SP5 STOP_1405</t>
+  </si>
+  <si>
+    <t>1_SP6 STOP_1405</t>
+  </si>
+  <si>
+    <t>1_SP7 STOP_1407</t>
+  </si>
+  <si>
+    <t>1_SP8 STOP_1408</t>
+  </si>
+  <si>
+    <t>1_SP9 STOP_ 1409</t>
+  </si>
+  <si>
+    <t>1_SP10 STOP_1410</t>
+  </si>
+  <si>
+    <t>1_SP11 STOP_1411</t>
+  </si>
+  <si>
+    <t>1_SP0 STOP_1420</t>
+  </si>
+  <si>
+    <t>PV FREQ MOTOR TRAVEL</t>
+  </si>
+  <si>
+    <t>PV CURRENT MOTOR TRAVEL</t>
+  </si>
+  <si>
+    <t>PV FREQ MOTOR LIFTER</t>
+  </si>
+  <si>
+    <t>PV CURRENT MOTOR LIFTER</t>
+  </si>
+  <si>
+    <t>PV TEMP MOTOR TRAVEL</t>
+  </si>
+  <si>
+    <t>PV TEMP MOTOR LIFTER</t>
+  </si>
+  <si>
+    <t>STOPPER-1 OPEN END</t>
+  </si>
+  <si>
+    <t>STOPPER-1 CLOSE END</t>
+  </si>
+  <si>
+    <t>STOPPER-2 OPEN END</t>
+  </si>
+  <si>
+    <t>STOPPER-2 CLOSE END</t>
+  </si>
+  <si>
+    <t>STOPPER-1 CLOSE</t>
+  </si>
+  <si>
+    <t>STOPPER-1 OPEN</t>
+  </si>
+  <si>
+    <t>POSITIONER-1 FORWARD</t>
+  </si>
+  <si>
+    <t>POSITIONER-1 REVERSE</t>
+  </si>
+  <si>
+    <t>STOPPER-3 CLOSE</t>
+  </si>
+  <si>
+    <t>STOPPER-3 OPEN</t>
+  </si>
+  <si>
+    <t>POSITIONER-3 FORWARD</t>
+  </si>
+  <si>
+    <t>POSITIONER-3 REVERSE</t>
+  </si>
+  <si>
+    <t>GUIDE CYL FWD RH</t>
+  </si>
+  <si>
+    <t>GUIDE CYL RVS RH</t>
+  </si>
+  <si>
+    <t>GUIDE CYL FWD LH</t>
+  </si>
+  <si>
+    <t>GUIDE CYL RVS LH</t>
+  </si>
+  <si>
+    <t>SOL GATE OPEN 1</t>
+  </si>
+  <si>
+    <t>SOL GATE CLOSE 1</t>
+  </si>
+  <si>
+    <t>SOL GATE CLOSE 2</t>
   </si>
 </sst>
 </file>
@@ -2128,8 +2503,11 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
@@ -2838,15 +3216,19 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
-  <dimension ref="A1:E162"/>
+  <dimension ref="A1:G162"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="M26" sqref="M26"/>
+      <selection activeCell="H9" sqref="H9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="5" max="5" width="17.33203125" customWidth="1"/>
+    <col min="6" max="6" width="35.6640625" bestFit="1" customWidth="1"/>
+  </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>27</v>
       </c>
@@ -2860,10 +3242,16 @@
         <v>30</v>
       </c>
       <c r="E1" t="s">
+        <v>686</v>
+      </c>
+      <c r="F1" t="s">
+        <v>687</v>
+      </c>
+      <c r="G1" t="s">
         <v>31</v>
       </c>
     </row>
-    <row r="2" spans="1:5" ht="17" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:7" ht="17" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>32</v>
       </c>
@@ -2876,11 +3264,17 @@
       <c r="D2" s="1" t="s">
         <v>132</v>
       </c>
-      <c r="E2" s="1">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="3" spans="1:5" ht="17" x14ac:dyDescent="0.2">
+      <c r="E2" s="2" t="s">
+        <v>711</v>
+      </c>
+      <c r="F2" s="2" t="s">
+        <v>688</v>
+      </c>
+      <c r="G2" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7" ht="17" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>35</v>
       </c>
@@ -2893,11 +3287,17 @@
       <c r="D3" s="1" t="s">
         <v>133</v>
       </c>
-      <c r="E3" s="1">
+      <c r="E3" s="2" t="s">
+        <v>712</v>
+      </c>
+      <c r="F3" s="2" t="s">
+        <v>689</v>
+      </c>
+      <c r="G3" s="1">
         <v>99</v>
       </c>
     </row>
-    <row r="4" spans="1:5" ht="17" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:7" ht="17" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>38</v>
       </c>
@@ -2910,11 +3310,17 @@
       <c r="D4" s="1" t="s">
         <v>134</v>
       </c>
-      <c r="E4" s="1">
+      <c r="E4" s="2" t="s">
+        <v>712</v>
+      </c>
+      <c r="F4" s="2" t="s">
+        <v>690</v>
+      </c>
+      <c r="G4" s="1">
         <v>56</v>
       </c>
     </row>
-    <row r="5" spans="1:5" ht="17" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:7" ht="17" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
         <v>51</v>
       </c>
@@ -2927,11 +3333,17 @@
       <c r="D5" s="1" t="s">
         <v>135</v>
       </c>
-      <c r="E5" s="1">
+      <c r="E5" s="2" t="s">
+        <v>712</v>
+      </c>
+      <c r="F5" s="2" t="s">
+        <v>691</v>
+      </c>
+      <c r="G5" s="1">
         <v>34</v>
       </c>
     </row>
-    <row r="6" spans="1:5" ht="17" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:7" ht="17" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
         <v>52</v>
       </c>
@@ -2944,11 +3356,17 @@
       <c r="D6" s="1" t="s">
         <v>136</v>
       </c>
-      <c r="E6" s="1">
+      <c r="E6" s="2" t="s">
+        <v>712</v>
+      </c>
+      <c r="F6" s="2" t="s">
+        <v>692</v>
+      </c>
+      <c r="G6" s="1">
         <v>51</v>
       </c>
     </row>
-    <row r="7" spans="1:5" ht="17" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:7" ht="17" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
         <v>53</v>
       </c>
@@ -2961,11 +3379,17 @@
       <c r="D7" s="1" t="s">
         <v>137</v>
       </c>
-      <c r="E7" s="1">
+      <c r="E7" s="2" t="s">
+        <v>712</v>
+      </c>
+      <c r="F7" s="2" t="s">
+        <v>693</v>
+      </c>
+      <c r="G7" s="1">
         <v>54</v>
       </c>
     </row>
-    <row r="8" spans="1:5" ht="17" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:7" ht="17" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
         <v>54</v>
       </c>
@@ -2978,11 +3402,17 @@
       <c r="D8" s="1" t="s">
         <v>138</v>
       </c>
-      <c r="E8" s="1">
+      <c r="E8" s="2" t="s">
+        <v>712</v>
+      </c>
+      <c r="F8" s="2" t="s">
+        <v>694</v>
+      </c>
+      <c r="G8" s="1">
         <v>52</v>
       </c>
     </row>
-    <row r="9" spans="1:5" ht="17" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:7" ht="17" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
         <v>55</v>
       </c>
@@ -2995,11 +3425,17 @@
       <c r="D9" s="1" t="s">
         <v>139</v>
       </c>
-      <c r="E9" s="1">
+      <c r="E9" s="2" t="s">
+        <v>712</v>
+      </c>
+      <c r="F9" s="2" t="s">
+        <v>695</v>
+      </c>
+      <c r="G9" s="1">
         <v>5</v>
       </c>
     </row>
-    <row r="10" spans="1:5" ht="17" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:7" ht="17" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
         <v>56</v>
       </c>
@@ -3012,11 +3448,17 @@
       <c r="D10" s="1" t="s">
         <v>140</v>
       </c>
-      <c r="E10" s="1">
+      <c r="E10" s="2" t="s">
+        <v>712</v>
+      </c>
+      <c r="F10" s="2" t="s">
+        <v>696</v>
+      </c>
+      <c r="G10" s="1">
         <v>4</v>
       </c>
     </row>
-    <row r="11" spans="1:5" ht="17" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:7" ht="17" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
         <v>57</v>
       </c>
@@ -3029,11 +3471,17 @@
       <c r="D11" s="1" t="s">
         <v>141</v>
       </c>
-      <c r="E11" s="1">
+      <c r="E11" s="2" t="s">
+        <v>712</v>
+      </c>
+      <c r="F11" s="2" t="s">
+        <v>697</v>
+      </c>
+      <c r="G11" s="1">
         <v>2</v>
       </c>
     </row>
-    <row r="12" spans="1:5" ht="17" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:7" ht="17" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
         <v>58</v>
       </c>
@@ -3046,11 +3494,17 @@
       <c r="D12" s="1" t="s">
         <v>142</v>
       </c>
-      <c r="E12" s="1">
+      <c r="E12" s="2" t="s">
+        <v>712</v>
+      </c>
+      <c r="F12" s="2" t="s">
+        <v>698</v>
+      </c>
+      <c r="G12" s="1">
         <v>2</v>
       </c>
     </row>
-    <row r="13" spans="1:5" ht="17" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:7" ht="17" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
         <v>59</v>
       </c>
@@ -3063,11 +3517,17 @@
       <c r="D13" s="1" t="s">
         <v>143</v>
       </c>
-      <c r="E13" s="1">
+      <c r="E13" s="2" t="s">
+        <v>712</v>
+      </c>
+      <c r="F13" s="2" t="s">
+        <v>699</v>
+      </c>
+      <c r="G13" s="1">
         <v>21</v>
       </c>
     </row>
-    <row r="14" spans="1:5" ht="17" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:7" ht="17" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
         <v>60</v>
       </c>
@@ -3080,11 +3540,17 @@
       <c r="D14" s="1" t="s">
         <v>144</v>
       </c>
-      <c r="E14" s="1">
+      <c r="E14" s="2" t="s">
+        <v>712</v>
+      </c>
+      <c r="F14" s="2" t="s">
+        <v>700</v>
+      </c>
+      <c r="G14" s="1">
         <v>67</v>
       </c>
     </row>
-    <row r="15" spans="1:5" ht="17" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:7" ht="17" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
         <v>61</v>
       </c>
@@ -3097,11 +3563,17 @@
       <c r="D15" s="1" t="s">
         <v>145</v>
       </c>
-      <c r="E15" s="1">
+      <c r="E15" s="2" t="s">
+        <v>712</v>
+      </c>
+      <c r="F15" s="2" t="s">
+        <v>701</v>
+      </c>
+      <c r="G15" s="1">
         <v>2</v>
       </c>
     </row>
-    <row r="16" spans="1:5" ht="17" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:7" ht="17" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
         <v>62</v>
       </c>
@@ -3114,11 +3586,17 @@
       <c r="D16" s="1" t="s">
         <v>146</v>
       </c>
-      <c r="E16" s="1">
+      <c r="E16" s="2" t="s">
+        <v>711</v>
+      </c>
+      <c r="F16" s="2" t="s">
+        <v>702</v>
+      </c>
+      <c r="G16" s="1">
         <v>1</v>
       </c>
     </row>
-    <row r="17" spans="1:5" ht="17" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:7" ht="17" x14ac:dyDescent="0.2">
       <c r="A17" t="s">
         <v>63</v>
       </c>
@@ -3131,11 +3609,17 @@
       <c r="D17" s="1" t="s">
         <v>147</v>
       </c>
-      <c r="E17" s="1">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="18" spans="1:5" ht="17" x14ac:dyDescent="0.2">
+      <c r="E17" s="2" t="s">
+        <v>711</v>
+      </c>
+      <c r="F17" s="2" t="s">
+        <v>703</v>
+      </c>
+      <c r="G17" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="18" spans="1:7" ht="17" x14ac:dyDescent="0.2">
       <c r="A18" t="s">
         <v>64</v>
       </c>
@@ -3148,11 +3632,17 @@
       <c r="D18" s="1" t="s">
         <v>148</v>
       </c>
-      <c r="E18" s="1">
+      <c r="E18" s="2" t="s">
+        <v>711</v>
+      </c>
+      <c r="F18" s="2" t="s">
+        <v>704</v>
+      </c>
+      <c r="G18" s="1">
         <v>1</v>
       </c>
     </row>
-    <row r="19" spans="1:5" ht="17" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:7" ht="17" x14ac:dyDescent="0.2">
       <c r="A19" t="s">
         <v>65</v>
       </c>
@@ -3165,11 +3655,17 @@
       <c r="D19" s="1" t="s">
         <v>149</v>
       </c>
-      <c r="E19" s="1">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="20" spans="1:5" ht="17" x14ac:dyDescent="0.2">
+      <c r="E19" s="2" t="s">
+        <v>711</v>
+      </c>
+      <c r="F19" s="2" t="s">
+        <v>705</v>
+      </c>
+      <c r="G19" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="20" spans="1:7" ht="17" x14ac:dyDescent="0.2">
       <c r="A20" t="s">
         <v>66</v>
       </c>
@@ -3182,11 +3678,17 @@
       <c r="D20" s="1" t="s">
         <v>150</v>
       </c>
-      <c r="E20" s="1">
+      <c r="E20" s="2" t="s">
+        <v>711</v>
+      </c>
+      <c r="F20" s="2" t="s">
+        <v>706</v>
+      </c>
+      <c r="G20" s="1">
         <v>1</v>
       </c>
     </row>
-    <row r="21" spans="1:5" ht="17" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:7" ht="17" x14ac:dyDescent="0.2">
       <c r="A21" t="s">
         <v>67</v>
       </c>
@@ -3199,11 +3701,17 @@
       <c r="D21" s="1" t="s">
         <v>151</v>
       </c>
-      <c r="E21" s="1">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="22" spans="1:5" ht="17" x14ac:dyDescent="0.2">
+      <c r="E21" s="2" t="s">
+        <v>711</v>
+      </c>
+      <c r="F21" s="2" t="s">
+        <v>707</v>
+      </c>
+      <c r="G21" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="22" spans="1:7" ht="17" x14ac:dyDescent="0.2">
       <c r="A22" t="s">
         <v>68</v>
       </c>
@@ -3216,11 +3724,17 @@
       <c r="D22" s="1" t="s">
         <v>152</v>
       </c>
-      <c r="E22" s="1">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="23" spans="1:5" ht="17" x14ac:dyDescent="0.2">
+      <c r="E22" s="2" t="s">
+        <v>711</v>
+      </c>
+      <c r="F22" s="2" t="s">
+        <v>708</v>
+      </c>
+      <c r="G22" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="23" spans="1:7" ht="17" x14ac:dyDescent="0.2">
       <c r="A23" t="s">
         <v>69</v>
       </c>
@@ -3233,11 +3747,17 @@
       <c r="D23" s="1" t="s">
         <v>153</v>
       </c>
-      <c r="E23" s="1">
+      <c r="E23" s="2" t="s">
+        <v>711</v>
+      </c>
+      <c r="F23" s="2" t="s">
+        <v>709</v>
+      </c>
+      <c r="G23" s="1">
         <v>1</v>
       </c>
     </row>
-    <row r="24" spans="1:5" ht="17" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:7" ht="17" x14ac:dyDescent="0.2">
       <c r="A24" t="s">
         <v>70</v>
       </c>
@@ -3250,11 +3770,17 @@
       <c r="D24" s="1" t="s">
         <v>154</v>
       </c>
-      <c r="E24" s="1">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="25" spans="1:5" ht="17" x14ac:dyDescent="0.2">
+      <c r="E24" s="2" t="s">
+        <v>711</v>
+      </c>
+      <c r="F24" s="2" t="s">
+        <v>710</v>
+      </c>
+      <c r="G24" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="25" spans="1:7" ht="17" x14ac:dyDescent="0.2">
       <c r="A25" t="s">
         <v>71</v>
       </c>
@@ -3267,11 +3793,17 @@
       <c r="D25" s="1" t="s">
         <v>155</v>
       </c>
-      <c r="E25" s="1">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="26" spans="1:5" ht="17" x14ac:dyDescent="0.2">
+      <c r="E25" s="2" t="s">
+        <v>711</v>
+      </c>
+      <c r="F25" s="2" t="s">
+        <v>714</v>
+      </c>
+      <c r="G25" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="26" spans="1:7" ht="17" x14ac:dyDescent="0.2">
       <c r="A26" t="s">
         <v>72</v>
       </c>
@@ -3284,11 +3816,17 @@
       <c r="D26" s="1" t="s">
         <v>156</v>
       </c>
-      <c r="E26" s="1">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="27" spans="1:5" ht="17" x14ac:dyDescent="0.2">
+      <c r="E26" s="2" t="s">
+        <v>711</v>
+      </c>
+      <c r="F26" s="2" t="s">
+        <v>715</v>
+      </c>
+      <c r="G26" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="27" spans="1:7" ht="17" x14ac:dyDescent="0.2">
       <c r="A27" t="s">
         <v>73</v>
       </c>
@@ -3301,11 +3839,17 @@
       <c r="D27" s="1" t="s">
         <v>157</v>
       </c>
-      <c r="E27" s="1">
+      <c r="E27" s="2" t="s">
+        <v>711</v>
+      </c>
+      <c r="F27" s="2" t="s">
+        <v>716</v>
+      </c>
+      <c r="G27" s="1">
         <v>1</v>
       </c>
     </row>
-    <row r="28" spans="1:5" ht="17" x14ac:dyDescent="0.2">
+    <row r="28" spans="1:7" ht="17" x14ac:dyDescent="0.2">
       <c r="A28" t="s">
         <v>74</v>
       </c>
@@ -3318,11 +3862,17 @@
       <c r="D28" s="1" t="s">
         <v>158</v>
       </c>
-      <c r="E28" s="1">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="29" spans="1:5" ht="17" x14ac:dyDescent="0.2">
+      <c r="E28" s="2" t="s">
+        <v>711</v>
+      </c>
+      <c r="F28" s="2" t="s">
+        <v>717</v>
+      </c>
+      <c r="G28" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="29" spans="1:7" ht="17" x14ac:dyDescent="0.2">
       <c r="A29" t="s">
         <v>75</v>
       </c>
@@ -3335,11 +3885,17 @@
       <c r="D29" s="1" t="s">
         <v>159</v>
       </c>
-      <c r="E29" s="1">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="30" spans="1:5" ht="17" x14ac:dyDescent="0.2">
+      <c r="E29" s="2" t="s">
+        <v>711</v>
+      </c>
+      <c r="F29" s="2" t="s">
+        <v>718</v>
+      </c>
+      <c r="G29" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="30" spans="1:7" ht="17" x14ac:dyDescent="0.2">
       <c r="A30" t="s">
         <v>76</v>
       </c>
@@ -3352,11 +3908,17 @@
       <c r="D30" s="1" t="s">
         <v>160</v>
       </c>
-      <c r="E30" s="1">
+      <c r="E30" s="2" t="s">
+        <v>711</v>
+      </c>
+      <c r="F30" s="2" t="s">
+        <v>719</v>
+      </c>
+      <c r="G30" s="1">
         <v>1</v>
       </c>
     </row>
-    <row r="31" spans="1:5" ht="17" x14ac:dyDescent="0.2">
+    <row r="31" spans="1:7" ht="17" x14ac:dyDescent="0.2">
       <c r="A31" t="s">
         <v>77</v>
       </c>
@@ -3369,11 +3931,17 @@
       <c r="D31" s="1" t="s">
         <v>161</v>
       </c>
-      <c r="E31" s="1">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="32" spans="1:5" ht="17" x14ac:dyDescent="0.2">
+      <c r="E31" s="2" t="s">
+        <v>711</v>
+      </c>
+      <c r="F31" s="2" t="s">
+        <v>720</v>
+      </c>
+      <c r="G31" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="32" spans="1:7" ht="17" x14ac:dyDescent="0.2">
       <c r="A32" t="s">
         <v>293</v>
       </c>
@@ -3386,11 +3954,17 @@
       <c r="D32" s="1" t="s">
         <v>162</v>
       </c>
-      <c r="E32" s="1">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="33" spans="1:5" ht="17" x14ac:dyDescent="0.2">
+      <c r="E32" s="2" t="s">
+        <v>711</v>
+      </c>
+      <c r="F32" s="2" t="s">
+        <v>721</v>
+      </c>
+      <c r="G32" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="33" spans="1:7" ht="17" x14ac:dyDescent="0.2">
       <c r="A33" t="s">
         <v>296</v>
       </c>
@@ -3403,11 +3977,17 @@
       <c r="D33" s="1" t="s">
         <v>163</v>
       </c>
-      <c r="E33" s="1">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="34" spans="1:5" ht="17" x14ac:dyDescent="0.2">
+      <c r="E33" s="2" t="s">
+        <v>711</v>
+      </c>
+      <c r="F33" s="2" t="s">
+        <v>722</v>
+      </c>
+      <c r="G33" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="34" spans="1:7" ht="17" x14ac:dyDescent="0.2">
       <c r="A34" t="s">
         <v>299</v>
       </c>
@@ -3420,11 +4000,17 @@
       <c r="D34" s="1" t="s">
         <v>164</v>
       </c>
-      <c r="E34" s="1">
+      <c r="E34" s="2" t="s">
+        <v>711</v>
+      </c>
+      <c r="F34" s="2" t="s">
+        <v>723</v>
+      </c>
+      <c r="G34" s="1">
         <v>1</v>
       </c>
     </row>
-    <row r="35" spans="1:5" ht="17" x14ac:dyDescent="0.2">
+    <row r="35" spans="1:7" ht="17" x14ac:dyDescent="0.2">
       <c r="A35" t="s">
         <v>302</v>
       </c>
@@ -3437,11 +4023,17 @@
       <c r="D35" s="1" t="s">
         <v>165</v>
       </c>
-      <c r="E35" s="1">
+      <c r="E35" s="2" t="s">
+        <v>711</v>
+      </c>
+      <c r="F35" s="2" t="s">
+        <v>724</v>
+      </c>
+      <c r="G35" s="1">
         <v>1</v>
       </c>
     </row>
-    <row r="36" spans="1:5" ht="17" x14ac:dyDescent="0.2">
+    <row r="36" spans="1:7" ht="17" x14ac:dyDescent="0.2">
       <c r="A36" t="s">
         <v>305</v>
       </c>
@@ -3454,11 +4046,17 @@
       <c r="D36" s="1" t="s">
         <v>166</v>
       </c>
-      <c r="E36" s="1">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="37" spans="1:5" ht="17" x14ac:dyDescent="0.2">
+      <c r="E36" s="2" t="s">
+        <v>711</v>
+      </c>
+      <c r="F36" s="2" t="s">
+        <v>725</v>
+      </c>
+      <c r="G36" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="37" spans="1:7" ht="17" x14ac:dyDescent="0.2">
       <c r="A37" t="s">
         <v>308</v>
       </c>
@@ -3471,11 +4069,17 @@
       <c r="D37" s="1" t="s">
         <v>167</v>
       </c>
-      <c r="E37" s="1">
+      <c r="E37" s="2" t="s">
+        <v>711</v>
+      </c>
+      <c r="F37" s="2" t="s">
+        <v>726</v>
+      </c>
+      <c r="G37" s="1">
         <v>1</v>
       </c>
     </row>
-    <row r="38" spans="1:5" ht="17" x14ac:dyDescent="0.2">
+    <row r="38" spans="1:7" ht="17" x14ac:dyDescent="0.2">
       <c r="A38" t="s">
         <v>311</v>
       </c>
@@ -3488,11 +4092,17 @@
       <c r="D38" s="1" t="s">
         <v>168</v>
       </c>
-      <c r="E38" s="1">
+      <c r="E38" s="2" t="s">
+        <v>711</v>
+      </c>
+      <c r="F38" s="2" t="s">
+        <v>727</v>
+      </c>
+      <c r="G38" s="1">
         <v>1</v>
       </c>
     </row>
-    <row r="39" spans="1:5" ht="17" x14ac:dyDescent="0.2">
+    <row r="39" spans="1:7" ht="17" x14ac:dyDescent="0.2">
       <c r="A39" t="s">
         <v>314</v>
       </c>
@@ -3505,11 +4115,17 @@
       <c r="D39" s="1" t="s">
         <v>169</v>
       </c>
-      <c r="E39" s="1">
+      <c r="E39" s="2" t="s">
+        <v>711</v>
+      </c>
+      <c r="F39" s="2" t="s">
+        <v>718</v>
+      </c>
+      <c r="G39" s="1">
         <v>1</v>
       </c>
     </row>
-    <row r="40" spans="1:5" ht="17" x14ac:dyDescent="0.2">
+    <row r="40" spans="1:7" ht="17" x14ac:dyDescent="0.2">
       <c r="A40" t="s">
         <v>317</v>
       </c>
@@ -3522,11 +4138,17 @@
       <c r="D40" s="1" t="s">
         <v>170</v>
       </c>
-      <c r="E40" s="1">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="41" spans="1:5" ht="17" x14ac:dyDescent="0.2">
+      <c r="E40" s="2" t="s">
+        <v>711</v>
+      </c>
+      <c r="F40" s="2" t="s">
+        <v>719</v>
+      </c>
+      <c r="G40" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="41" spans="1:7" ht="17" x14ac:dyDescent="0.2">
       <c r="A41" t="s">
         <v>320</v>
       </c>
@@ -3539,11 +4161,17 @@
       <c r="D41" s="1" t="s">
         <v>171</v>
       </c>
-      <c r="E41" s="1">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="42" spans="1:5" ht="17" x14ac:dyDescent="0.2">
+      <c r="E41" s="2" t="s">
+        <v>711</v>
+      </c>
+      <c r="F41" s="2" t="s">
+        <v>720</v>
+      </c>
+      <c r="G41" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="42" spans="1:7" ht="17" x14ac:dyDescent="0.2">
       <c r="A42" t="s">
         <v>323</v>
       </c>
@@ -3556,11 +4184,17 @@
       <c r="D42" s="1" t="s">
         <v>172</v>
       </c>
-      <c r="E42" s="1">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="43" spans="1:5" ht="17" x14ac:dyDescent="0.2">
+      <c r="E42" s="2" t="s">
+        <v>711</v>
+      </c>
+      <c r="F42" s="2" t="s">
+        <v>728</v>
+      </c>
+      <c r="G42" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="43" spans="1:7" ht="17" x14ac:dyDescent="0.2">
       <c r="A43" t="s">
         <v>326</v>
       </c>
@@ -3573,11 +4207,17 @@
       <c r="D43" s="1" t="s">
         <v>173</v>
       </c>
-      <c r="E43" s="1">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="44" spans="1:5" ht="17" x14ac:dyDescent="0.2">
+      <c r="E43" s="2" t="s">
+        <v>711</v>
+      </c>
+      <c r="F43" s="2" t="s">
+        <v>721</v>
+      </c>
+      <c r="G43" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="44" spans="1:7" ht="17" x14ac:dyDescent="0.2">
       <c r="A44" t="s">
         <v>329</v>
       </c>
@@ -3590,11 +4230,17 @@
       <c r="D44" s="1" t="s">
         <v>174</v>
       </c>
-      <c r="E44" s="1">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="45" spans="1:5" ht="17" x14ac:dyDescent="0.2">
+      <c r="E44" s="2" t="s">
+        <v>711</v>
+      </c>
+      <c r="F44" s="2" t="s">
+        <v>722</v>
+      </c>
+      <c r="G44" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="45" spans="1:7" ht="17" x14ac:dyDescent="0.2">
       <c r="A45" t="s">
         <v>332</v>
       </c>
@@ -3607,11 +4253,17 @@
       <c r="D45" s="1" t="s">
         <v>175</v>
       </c>
-      <c r="E45" s="1">
+      <c r="E45" s="2" t="s">
+        <v>711</v>
+      </c>
+      <c r="F45" s="2" t="s">
+        <v>729</v>
+      </c>
+      <c r="G45" s="1">
         <v>1</v>
       </c>
     </row>
-    <row r="46" spans="1:5" ht="17" x14ac:dyDescent="0.2">
+    <row r="46" spans="1:7" ht="17" x14ac:dyDescent="0.2">
       <c r="A46" t="s">
         <v>335</v>
       </c>
@@ -3624,11 +4276,17 @@
       <c r="D46" s="1" t="s">
         <v>176</v>
       </c>
-      <c r="E46" s="1">
+      <c r="E46" s="2" t="s">
+        <v>711</v>
+      </c>
+      <c r="F46" s="2" t="s">
+        <v>730</v>
+      </c>
+      <c r="G46" s="1">
         <v>1</v>
       </c>
     </row>
-    <row r="47" spans="1:5" ht="17" x14ac:dyDescent="0.2">
+    <row r="47" spans="1:7" ht="17" x14ac:dyDescent="0.2">
       <c r="A47" t="s">
         <v>338</v>
       </c>
@@ -3641,11 +4299,17 @@
       <c r="D47" s="1" t="s">
         <v>177</v>
       </c>
-      <c r="E47" s="1">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="48" spans="1:5" ht="17" x14ac:dyDescent="0.2">
+      <c r="E47" s="2" t="s">
+        <v>711</v>
+      </c>
+      <c r="F47" s="2" t="s">
+        <v>731</v>
+      </c>
+      <c r="G47" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="48" spans="1:7" ht="17" x14ac:dyDescent="0.2">
       <c r="A48" t="s">
         <v>341</v>
       </c>
@@ -3658,11 +4322,17 @@
       <c r="D48" s="1" t="s">
         <v>178</v>
       </c>
-      <c r="E48" s="1">
+      <c r="E48" s="2" t="s">
+        <v>711</v>
+      </c>
+      <c r="F48" s="2" t="s">
+        <v>732</v>
+      </c>
+      <c r="G48" s="1">
         <v>1</v>
       </c>
     </row>
-    <row r="49" spans="1:5" ht="17" x14ac:dyDescent="0.2">
+    <row r="49" spans="1:7" ht="17" x14ac:dyDescent="0.2">
       <c r="A49" t="s">
         <v>344</v>
       </c>
@@ -3675,11 +4345,17 @@
       <c r="D49" s="1" t="s">
         <v>179</v>
       </c>
-      <c r="E49" s="1">
+      <c r="E49" s="2" t="s">
+        <v>711</v>
+      </c>
+      <c r="F49" s="2" t="s">
+        <v>733</v>
+      </c>
+      <c r="G49" s="1">
         <v>1</v>
       </c>
     </row>
-    <row r="50" spans="1:5" ht="17" x14ac:dyDescent="0.2">
+    <row r="50" spans="1:7" ht="17" x14ac:dyDescent="0.2">
       <c r="A50" t="s">
         <v>347</v>
       </c>
@@ -3692,11 +4368,17 @@
       <c r="D50" s="1" t="s">
         <v>180</v>
       </c>
-      <c r="E50" s="1">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="51" spans="1:5" ht="17" x14ac:dyDescent="0.2">
+      <c r="E50" s="2" t="s">
+        <v>711</v>
+      </c>
+      <c r="F50" s="2" t="s">
+        <v>734</v>
+      </c>
+      <c r="G50" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="51" spans="1:7" ht="17" x14ac:dyDescent="0.2">
       <c r="A51" t="s">
         <v>350</v>
       </c>
@@ -3709,11 +4391,17 @@
       <c r="D51" s="1" t="s">
         <v>181</v>
       </c>
-      <c r="E51" s="1">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="52" spans="1:5" ht="17" x14ac:dyDescent="0.2">
+      <c r="E51" s="2" t="s">
+        <v>711</v>
+      </c>
+      <c r="F51" s="2" t="s">
+        <v>735</v>
+      </c>
+      <c r="G51" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="52" spans="1:7" ht="17" x14ac:dyDescent="0.2">
       <c r="A52" t="s">
         <v>353</v>
       </c>
@@ -3726,11 +4414,17 @@
       <c r="D52" s="1" t="s">
         <v>182</v>
       </c>
-      <c r="E52" s="1">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="53" spans="1:5" ht="17" x14ac:dyDescent="0.2">
+      <c r="E52" s="2" t="s">
+        <v>711</v>
+      </c>
+      <c r="F52" s="2" t="s">
+        <v>736</v>
+      </c>
+      <c r="G52" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="53" spans="1:7" ht="17" x14ac:dyDescent="0.2">
       <c r="A53" t="s">
         <v>356</v>
       </c>
@@ -3743,11 +4437,17 @@
       <c r="D53" s="1" t="s">
         <v>183</v>
       </c>
-      <c r="E53" s="1">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="54" spans="1:5" ht="17" x14ac:dyDescent="0.2">
+      <c r="E53" s="2" t="s">
+        <v>711</v>
+      </c>
+      <c r="F53" s="2" t="s">
+        <v>737</v>
+      </c>
+      <c r="G53" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="54" spans="1:7" ht="17" x14ac:dyDescent="0.2">
       <c r="A54" t="s">
         <v>359</v>
       </c>
@@ -3760,11 +4460,17 @@
       <c r="D54" s="1" t="s">
         <v>184</v>
       </c>
-      <c r="E54" s="1">
+      <c r="E54" s="2" t="s">
+        <v>711</v>
+      </c>
+      <c r="F54" s="2" t="s">
+        <v>738</v>
+      </c>
+      <c r="G54" s="1">
         <v>1</v>
       </c>
     </row>
-    <row r="55" spans="1:5" ht="17" x14ac:dyDescent="0.2">
+    <row r="55" spans="1:7" ht="17" x14ac:dyDescent="0.2">
       <c r="A55" t="s">
         <v>362</v>
       </c>
@@ -3777,11 +4483,17 @@
       <c r="D55" s="1" t="s">
         <v>185</v>
       </c>
-      <c r="E55" s="1">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="56" spans="1:5" ht="17" x14ac:dyDescent="0.2">
+      <c r="E55" s="2" t="s">
+        <v>711</v>
+      </c>
+      <c r="F55" s="2" t="s">
+        <v>739</v>
+      </c>
+      <c r="G55" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="56" spans="1:7" ht="17" x14ac:dyDescent="0.2">
       <c r="A56" t="s">
         <v>365</v>
       </c>
@@ -3794,11 +4506,17 @@
       <c r="D56" s="1" t="s">
         <v>186</v>
       </c>
-      <c r="E56" s="1">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="57" spans="1:5" ht="17" x14ac:dyDescent="0.2">
+      <c r="E56" s="2" t="s">
+        <v>711</v>
+      </c>
+      <c r="F56" s="2" t="s">
+        <v>740</v>
+      </c>
+      <c r="G56" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="57" spans="1:7" ht="17" x14ac:dyDescent="0.2">
       <c r="A57" t="s">
         <v>368</v>
       </c>
@@ -3811,11 +4529,17 @@
       <c r="D57" s="1" t="s">
         <v>187</v>
       </c>
-      <c r="E57" s="1">
+      <c r="E57" s="2" t="s">
+        <v>711</v>
+      </c>
+      <c r="F57" s="2" t="s">
+        <v>741</v>
+      </c>
+      <c r="G57" s="1">
         <v>1</v>
       </c>
     </row>
-    <row r="58" spans="1:5" ht="17" x14ac:dyDescent="0.2">
+    <row r="58" spans="1:7" ht="17" x14ac:dyDescent="0.2">
       <c r="A58" t="s">
         <v>371</v>
       </c>
@@ -3828,11 +4552,17 @@
       <c r="D58" s="1" t="s">
         <v>188</v>
       </c>
-      <c r="E58" s="1">
+      <c r="E58" s="2" t="s">
+        <v>711</v>
+      </c>
+      <c r="F58" s="2" t="s">
+        <v>742</v>
+      </c>
+      <c r="G58" s="1">
         <v>1</v>
       </c>
     </row>
-    <row r="59" spans="1:5" ht="17" x14ac:dyDescent="0.2">
+    <row r="59" spans="1:7" ht="17" x14ac:dyDescent="0.2">
       <c r="A59" t="s">
         <v>374</v>
       </c>
@@ -3845,11 +4575,17 @@
       <c r="D59" s="1" t="s">
         <v>189</v>
       </c>
-      <c r="E59" s="1">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="60" spans="1:5" ht="17" x14ac:dyDescent="0.2">
+      <c r="E59" s="2" t="s">
+        <v>711</v>
+      </c>
+      <c r="F59" s="2" t="s">
+        <v>743</v>
+      </c>
+      <c r="G59" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="60" spans="1:7" ht="17" x14ac:dyDescent="0.2">
       <c r="A60" t="s">
         <v>377</v>
       </c>
@@ -3862,11 +4598,17 @@
       <c r="D60" s="1" t="s">
         <v>190</v>
       </c>
-      <c r="E60" s="1">
+      <c r="E60" s="2" t="s">
+        <v>711</v>
+      </c>
+      <c r="F60" s="2" t="s">
+        <v>744</v>
+      </c>
+      <c r="G60" s="1">
         <v>1</v>
       </c>
     </row>
-    <row r="61" spans="1:5" ht="17" x14ac:dyDescent="0.2">
+    <row r="61" spans="1:7" ht="17" x14ac:dyDescent="0.2">
       <c r="A61" t="s">
         <v>380</v>
       </c>
@@ -3879,11 +4621,17 @@
       <c r="D61" s="1" t="s">
         <v>191</v>
       </c>
-      <c r="E61" s="1">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="62" spans="1:5" ht="17" x14ac:dyDescent="0.2">
+      <c r="E61" s="2" t="s">
+        <v>711</v>
+      </c>
+      <c r="F61" s="2" t="s">
+        <v>745</v>
+      </c>
+      <c r="G61" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="62" spans="1:7" ht="17" x14ac:dyDescent="0.2">
       <c r="A62" t="s">
         <v>383</v>
       </c>
@@ -3896,11 +4644,17 @@
       <c r="D62" s="1" t="s">
         <v>192</v>
       </c>
-      <c r="E62" s="1">
+      <c r="E62" s="2" t="s">
+        <v>711</v>
+      </c>
+      <c r="F62" s="2" t="s">
+        <v>746</v>
+      </c>
+      <c r="G62" s="1">
         <v>1</v>
       </c>
     </row>
-    <row r="63" spans="1:5" ht="17" x14ac:dyDescent="0.2">
+    <row r="63" spans="1:7" ht="17" x14ac:dyDescent="0.2">
       <c r="A63" t="s">
         <v>386</v>
       </c>
@@ -3913,11 +4667,17 @@
       <c r="D63" s="1" t="s">
         <v>193</v>
       </c>
-      <c r="E63" s="1">
+      <c r="E63" s="2" t="s">
+        <v>711</v>
+      </c>
+      <c r="F63" s="2" t="s">
+        <v>747</v>
+      </c>
+      <c r="G63" s="1">
         <v>1</v>
       </c>
     </row>
-    <row r="64" spans="1:5" ht="17" x14ac:dyDescent="0.2">
+    <row r="64" spans="1:7" ht="17" x14ac:dyDescent="0.2">
       <c r="A64" t="s">
         <v>389</v>
       </c>
@@ -3930,11 +4690,17 @@
       <c r="D64" s="1" t="s">
         <v>194</v>
       </c>
-      <c r="E64" s="1">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="65" spans="1:5" ht="17" x14ac:dyDescent="0.2">
+      <c r="E64" s="2" t="s">
+        <v>711</v>
+      </c>
+      <c r="F64" s="2" t="s">
+        <v>748</v>
+      </c>
+      <c r="G64" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="65" spans="1:7" ht="17" x14ac:dyDescent="0.2">
       <c r="A65" t="s">
         <v>392</v>
       </c>
@@ -3947,11 +4713,17 @@
       <c r="D65" s="1" t="s">
         <v>195</v>
       </c>
-      <c r="E65" s="1">
+      <c r="E65" s="2" t="s">
+        <v>711</v>
+      </c>
+      <c r="F65" s="2" t="s">
+        <v>749</v>
+      </c>
+      <c r="G65" s="1">
         <v>1</v>
       </c>
     </row>
-    <row r="66" spans="1:5" ht="17" x14ac:dyDescent="0.2">
+    <row r="66" spans="1:7" ht="17" x14ac:dyDescent="0.2">
       <c r="A66" t="s">
         <v>395</v>
       </c>
@@ -3964,11 +4736,17 @@
       <c r="D66" s="1" t="s">
         <v>196</v>
       </c>
-      <c r="E66" s="1">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="67" spans="1:5" ht="17" x14ac:dyDescent="0.2">
+      <c r="E66" s="2" t="s">
+        <v>711</v>
+      </c>
+      <c r="F66" s="2" t="s">
+        <v>750</v>
+      </c>
+      <c r="G66" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="67" spans="1:7" ht="17" x14ac:dyDescent="0.2">
       <c r="A67" t="s">
         <v>398</v>
       </c>
@@ -3981,11 +4759,17 @@
       <c r="D67" s="1" t="s">
         <v>197</v>
       </c>
-      <c r="E67" s="1">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="68" spans="1:5" ht="17" x14ac:dyDescent="0.2">
+      <c r="E67" s="2" t="s">
+        <v>711</v>
+      </c>
+      <c r="F67" s="2" t="s">
+        <v>751</v>
+      </c>
+      <c r="G67" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="68" spans="1:7" ht="17" x14ac:dyDescent="0.2">
       <c r="A68" t="s">
         <v>401</v>
       </c>
@@ -3998,11 +4782,17 @@
       <c r="D68" s="1" t="s">
         <v>198</v>
       </c>
-      <c r="E68" s="1">
+      <c r="E68" s="2" t="s">
+        <v>711</v>
+      </c>
+      <c r="F68" s="2" t="s">
+        <v>752</v>
+      </c>
+      <c r="G68" s="1">
         <v>1</v>
       </c>
     </row>
-    <row r="69" spans="1:5" ht="17" x14ac:dyDescent="0.2">
+    <row r="69" spans="1:7" ht="17" x14ac:dyDescent="0.2">
       <c r="A69" t="s">
         <v>404</v>
       </c>
@@ -4015,11 +4805,17 @@
       <c r="D69" s="1" t="s">
         <v>199</v>
       </c>
-      <c r="E69" s="1">
+      <c r="E69" s="2" t="s">
+        <v>711</v>
+      </c>
+      <c r="F69" s="2" t="s">
+        <v>753</v>
+      </c>
+      <c r="G69" s="1">
         <v>1</v>
       </c>
     </row>
-    <row r="70" spans="1:5" ht="17" x14ac:dyDescent="0.2">
+    <row r="70" spans="1:7" ht="17" x14ac:dyDescent="0.2">
       <c r="A70" t="s">
         <v>407</v>
       </c>
@@ -4032,11 +4828,17 @@
       <c r="D70" s="1" t="s">
         <v>200</v>
       </c>
-      <c r="E70" s="1">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="71" spans="1:5" ht="17" x14ac:dyDescent="0.2">
+      <c r="E70" s="2" t="s">
+        <v>711</v>
+      </c>
+      <c r="F70" s="2" t="s">
+        <v>754</v>
+      </c>
+      <c r="G70" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="71" spans="1:7" ht="17" x14ac:dyDescent="0.2">
       <c r="A71" t="s">
         <v>410</v>
       </c>
@@ -4049,11 +4851,17 @@
       <c r="D71" s="1" t="s">
         <v>201</v>
       </c>
-      <c r="E71" s="1">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="72" spans="1:5" ht="17" x14ac:dyDescent="0.2">
+      <c r="E71" s="2" t="s">
+        <v>711</v>
+      </c>
+      <c r="F71" s="2" t="s">
+        <v>755</v>
+      </c>
+      <c r="G71" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="72" spans="1:7" ht="17" x14ac:dyDescent="0.2">
       <c r="A72" t="s">
         <v>413</v>
       </c>
@@ -4066,11 +4874,17 @@
       <c r="D72" s="1" t="s">
         <v>202</v>
       </c>
-      <c r="E72" s="1">
+      <c r="E72" s="2" t="s">
+        <v>711</v>
+      </c>
+      <c r="F72" s="2" t="s">
+        <v>756</v>
+      </c>
+      <c r="G72" s="1">
         <v>1</v>
       </c>
     </row>
-    <row r="73" spans="1:5" ht="17" x14ac:dyDescent="0.2">
+    <row r="73" spans="1:7" ht="17" x14ac:dyDescent="0.2">
       <c r="A73" t="s">
         <v>416</v>
       </c>
@@ -4083,11 +4897,17 @@
       <c r="D73" s="1" t="s">
         <v>203</v>
       </c>
-      <c r="E73" s="1">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="74" spans="1:5" ht="17" x14ac:dyDescent="0.2">
+      <c r="E73" s="2" t="s">
+        <v>711</v>
+      </c>
+      <c r="F73" s="2" t="s">
+        <v>757</v>
+      </c>
+      <c r="G73" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="74" spans="1:7" ht="17" x14ac:dyDescent="0.2">
       <c r="A74" t="s">
         <v>419</v>
       </c>
@@ -4100,11 +4920,17 @@
       <c r="D74" s="1" t="s">
         <v>204</v>
       </c>
-      <c r="E74" s="1">
+      <c r="E74" s="2" t="s">
+        <v>711</v>
+      </c>
+      <c r="F74" s="2" t="s">
+        <v>758</v>
+      </c>
+      <c r="G74" s="1">
         <v>1</v>
       </c>
     </row>
-    <row r="75" spans="1:5" ht="17" x14ac:dyDescent="0.2">
+    <row r="75" spans="1:7" ht="17" x14ac:dyDescent="0.2">
       <c r="A75" t="s">
         <v>422</v>
       </c>
@@ -4117,11 +4943,17 @@
       <c r="D75" s="1" t="s">
         <v>205</v>
       </c>
-      <c r="E75" s="1">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="76" spans="1:5" ht="17" x14ac:dyDescent="0.2">
+      <c r="E75" s="2" t="s">
+        <v>711</v>
+      </c>
+      <c r="F75" s="2" t="s">
+        <v>759</v>
+      </c>
+      <c r="G75" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="76" spans="1:7" ht="17" x14ac:dyDescent="0.2">
       <c r="A76" t="s">
         <v>425</v>
       </c>
@@ -4134,11 +4966,17 @@
       <c r="D76" s="1" t="s">
         <v>206</v>
       </c>
-      <c r="E76" s="1">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="77" spans="1:5" ht="17" x14ac:dyDescent="0.2">
+      <c r="E76" s="2" t="s">
+        <v>711</v>
+      </c>
+      <c r="F76" s="2" t="s">
+        <v>760</v>
+      </c>
+      <c r="G76" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="77" spans="1:7" ht="17" x14ac:dyDescent="0.2">
       <c r="A77" t="s">
         <v>428</v>
       </c>
@@ -4151,11 +4989,17 @@
       <c r="D77" s="1" t="s">
         <v>207</v>
       </c>
-      <c r="E77" s="1">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="78" spans="1:5" ht="17" x14ac:dyDescent="0.2">
+      <c r="E77" s="2" t="s">
+        <v>711</v>
+      </c>
+      <c r="F77" s="2" t="s">
+        <v>761</v>
+      </c>
+      <c r="G77" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="78" spans="1:7" ht="17" x14ac:dyDescent="0.2">
       <c r="A78" t="s">
         <v>431</v>
       </c>
@@ -4168,11 +5012,17 @@
       <c r="D78" s="1" t="s">
         <v>208</v>
       </c>
-      <c r="E78" s="1">
+      <c r="E78" s="2" t="s">
+        <v>711</v>
+      </c>
+      <c r="F78" s="2" t="s">
+        <v>762</v>
+      </c>
+      <c r="G78" s="1">
         <v>1</v>
       </c>
     </row>
-    <row r="79" spans="1:5" ht="17" x14ac:dyDescent="0.2">
+    <row r="79" spans="1:7" ht="17" x14ac:dyDescent="0.2">
       <c r="A79" t="s">
         <v>434</v>
       </c>
@@ -4185,11 +5035,17 @@
       <c r="D79" s="1" t="s">
         <v>209</v>
       </c>
-      <c r="E79" s="1">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="80" spans="1:5" ht="17" x14ac:dyDescent="0.2">
+      <c r="E79" s="2" t="s">
+        <v>711</v>
+      </c>
+      <c r="F79" s="2" t="s">
+        <v>763</v>
+      </c>
+      <c r="G79" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="80" spans="1:7" ht="17" x14ac:dyDescent="0.2">
       <c r="A80" t="s">
         <v>437</v>
       </c>
@@ -4202,11 +5058,17 @@
       <c r="D80" s="1" t="s">
         <v>210</v>
       </c>
-      <c r="E80" s="1">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="81" spans="1:5" ht="17" x14ac:dyDescent="0.2">
+      <c r="E80" s="2" t="s">
+        <v>711</v>
+      </c>
+      <c r="F80" s="2" t="s">
+        <v>764</v>
+      </c>
+      <c r="G80" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="81" spans="1:7" ht="17" x14ac:dyDescent="0.2">
       <c r="A81" t="s">
         <v>440</v>
       </c>
@@ -4219,11 +5081,17 @@
       <c r="D81" s="1" t="s">
         <v>211</v>
       </c>
-      <c r="E81" s="1">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="82" spans="1:5" ht="17" x14ac:dyDescent="0.2">
+      <c r="E81" s="2" t="s">
+        <v>711</v>
+      </c>
+      <c r="F81" s="2" t="s">
+        <v>765</v>
+      </c>
+      <c r="G81" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="82" spans="1:7" ht="17" x14ac:dyDescent="0.2">
       <c r="A82" t="s">
         <v>443</v>
       </c>
@@ -4236,11 +5104,17 @@
       <c r="D82" s="1" t="s">
         <v>212</v>
       </c>
-      <c r="E82" s="1">
+      <c r="E82" s="2" t="s">
+        <v>711</v>
+      </c>
+      <c r="F82" s="2" t="s">
+        <v>766</v>
+      </c>
+      <c r="G82" s="1">
         <v>1</v>
       </c>
     </row>
-    <row r="83" spans="1:5" ht="17" x14ac:dyDescent="0.2">
+    <row r="83" spans="1:7" ht="17" x14ac:dyDescent="0.2">
       <c r="A83" t="s">
         <v>446</v>
       </c>
@@ -4253,11 +5127,17 @@
       <c r="D83" s="1" t="s">
         <v>213</v>
       </c>
-      <c r="E83" s="1">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="84" spans="1:5" ht="17" x14ac:dyDescent="0.2">
+      <c r="E83" s="2" t="s">
+        <v>711</v>
+      </c>
+      <c r="F83" s="2" t="s">
+        <v>767</v>
+      </c>
+      <c r="G83" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="84" spans="1:7" ht="17" x14ac:dyDescent="0.2">
       <c r="A84" t="s">
         <v>449</v>
       </c>
@@ -4270,11 +5150,17 @@
       <c r="D84" s="1" t="s">
         <v>214</v>
       </c>
-      <c r="E84" s="1">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="85" spans="1:5" ht="17" x14ac:dyDescent="0.2">
+      <c r="E84" s="2" t="s">
+        <v>711</v>
+      </c>
+      <c r="F84" s="2" t="s">
+        <v>768</v>
+      </c>
+      <c r="G84" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="85" spans="1:7" ht="17" x14ac:dyDescent="0.2">
       <c r="A85" t="s">
         <v>452</v>
       </c>
@@ -4287,11 +5173,17 @@
       <c r="D85" s="1" t="s">
         <v>215</v>
       </c>
-      <c r="E85" s="1">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="86" spans="1:5" ht="17" x14ac:dyDescent="0.2">
+      <c r="E85" s="2" t="s">
+        <v>711</v>
+      </c>
+      <c r="F85" s="2" t="s">
+        <v>769</v>
+      </c>
+      <c r="G85" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="86" spans="1:7" ht="17" x14ac:dyDescent="0.2">
       <c r="A86" t="s">
         <v>455</v>
       </c>
@@ -4304,11 +5196,17 @@
       <c r="D86" s="1" t="s">
         <v>216</v>
       </c>
-      <c r="E86" s="1">
+      <c r="E86" s="2" t="s">
+        <v>711</v>
+      </c>
+      <c r="F86" s="2" t="s">
+        <v>770</v>
+      </c>
+      <c r="G86" s="1">
         <v>1</v>
       </c>
     </row>
-    <row r="87" spans="1:5" ht="17" x14ac:dyDescent="0.2">
+    <row r="87" spans="1:7" ht="17" x14ac:dyDescent="0.2">
       <c r="A87" t="s">
         <v>458</v>
       </c>
@@ -4321,11 +5219,17 @@
       <c r="D87" s="1" t="s">
         <v>217</v>
       </c>
-      <c r="E87" s="1">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="88" spans="1:5" ht="17" x14ac:dyDescent="0.2">
+      <c r="E87" s="2" t="s">
+        <v>711</v>
+      </c>
+      <c r="F87" s="2" t="s">
+        <v>771</v>
+      </c>
+      <c r="G87" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="88" spans="1:7" ht="17" x14ac:dyDescent="0.2">
       <c r="A88" t="s">
         <v>461</v>
       </c>
@@ -4338,11 +5242,17 @@
       <c r="D88" s="1" t="s">
         <v>218</v>
       </c>
-      <c r="E88" s="1">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="89" spans="1:5" ht="17" x14ac:dyDescent="0.2">
+      <c r="E88" s="2" t="s">
+        <v>711</v>
+      </c>
+      <c r="F88" s="2" t="s">
+        <v>772</v>
+      </c>
+      <c r="G88" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="89" spans="1:7" ht="34" x14ac:dyDescent="0.2">
       <c r="A89" t="s">
         <v>464</v>
       </c>
@@ -4355,11 +5265,17 @@
       <c r="D89" s="1" t="s">
         <v>219</v>
       </c>
-      <c r="E89" s="1">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="90" spans="1:5" ht="17" x14ac:dyDescent="0.2">
+      <c r="E89" s="2" t="s">
+        <v>711</v>
+      </c>
+      <c r="F89" s="2" t="s">
+        <v>773</v>
+      </c>
+      <c r="G89" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="90" spans="1:7" ht="17" x14ac:dyDescent="0.2">
       <c r="A90" t="s">
         <v>467</v>
       </c>
@@ -4372,11 +5288,17 @@
       <c r="D90" s="1" t="s">
         <v>220</v>
       </c>
-      <c r="E90" s="1">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="91" spans="1:5" ht="17" x14ac:dyDescent="0.2">
+      <c r="E90" s="2" t="s">
+        <v>711</v>
+      </c>
+      <c r="F90" s="2" t="s">
+        <v>774</v>
+      </c>
+      <c r="G90" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="91" spans="1:7" ht="17" x14ac:dyDescent="0.2">
       <c r="A91" t="s">
         <v>470</v>
       </c>
@@ -4389,11 +5311,17 @@
       <c r="D91" s="1" t="s">
         <v>221</v>
       </c>
-      <c r="E91" s="1">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="92" spans="1:5" ht="17" x14ac:dyDescent="0.2">
+      <c r="E91" s="2" t="s">
+        <v>711</v>
+      </c>
+      <c r="F91" s="2" t="s">
+        <v>775</v>
+      </c>
+      <c r="G91" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="92" spans="1:7" ht="17" x14ac:dyDescent="0.2">
       <c r="A92" t="s">
         <v>473</v>
       </c>
@@ -4406,11 +5334,17 @@
       <c r="D92" s="1" t="s">
         <v>222</v>
       </c>
-      <c r="E92" s="1">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="93" spans="1:5" ht="17" x14ac:dyDescent="0.2">
+      <c r="E92" s="2" t="s">
+        <v>711</v>
+      </c>
+      <c r="F92" s="2" t="s">
+        <v>776</v>
+      </c>
+      <c r="G92" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="93" spans="1:7" ht="17" x14ac:dyDescent="0.2">
       <c r="A93" t="s">
         <v>476</v>
       </c>
@@ -4423,11 +5357,17 @@
       <c r="D93" s="1" t="s">
         <v>223</v>
       </c>
-      <c r="E93" s="1">
+      <c r="E93" s="2" t="s">
+        <v>711</v>
+      </c>
+      <c r="F93" s="2" t="s">
+        <v>777</v>
+      </c>
+      <c r="G93" s="1">
         <v>1</v>
       </c>
     </row>
-    <row r="94" spans="1:5" ht="17" x14ac:dyDescent="0.2">
+    <row r="94" spans="1:7" ht="17" x14ac:dyDescent="0.2">
       <c r="A94" t="s">
         <v>479</v>
       </c>
@@ -4440,11 +5380,17 @@
       <c r="D94" s="1" t="s">
         <v>224</v>
       </c>
-      <c r="E94" s="1">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="95" spans="1:5" ht="17" x14ac:dyDescent="0.2">
+      <c r="E94" s="2" t="s">
+        <v>711</v>
+      </c>
+      <c r="F94" s="2" t="s">
+        <v>778</v>
+      </c>
+      <c r="G94" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="95" spans="1:7" ht="17" x14ac:dyDescent="0.2">
       <c r="A95" t="s">
         <v>482</v>
       </c>
@@ -4457,11 +5403,17 @@
       <c r="D95" s="1" t="s">
         <v>225</v>
       </c>
-      <c r="E95" s="1">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="96" spans="1:5" ht="17" x14ac:dyDescent="0.2">
+      <c r="E95" s="2" t="s">
+        <v>711</v>
+      </c>
+      <c r="F95" s="2" t="s">
+        <v>779</v>
+      </c>
+      <c r="G95" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="96" spans="1:7" ht="17" x14ac:dyDescent="0.2">
       <c r="A96" t="s">
         <v>485</v>
       </c>
@@ -4474,11 +5426,17 @@
       <c r="D96" s="1" t="s">
         <v>226</v>
       </c>
-      <c r="E96" s="1">
+      <c r="E96" s="2" t="s">
+        <v>711</v>
+      </c>
+      <c r="F96" s="2" t="s">
+        <v>780</v>
+      </c>
+      <c r="G96" s="1">
         <v>1</v>
       </c>
     </row>
-    <row r="97" spans="1:5" ht="17" x14ac:dyDescent="0.2">
+    <row r="97" spans="1:7" ht="17" x14ac:dyDescent="0.2">
       <c r="A97" t="s">
         <v>488</v>
       </c>
@@ -4491,11 +5449,17 @@
       <c r="D97" s="1" t="s">
         <v>227</v>
       </c>
-      <c r="E97" s="1">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="98" spans="1:5" ht="17" x14ac:dyDescent="0.2">
+      <c r="E97" s="2" t="s">
+        <v>711</v>
+      </c>
+      <c r="F97" s="2" t="s">
+        <v>781</v>
+      </c>
+      <c r="G97" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="98" spans="1:7" ht="17" x14ac:dyDescent="0.2">
       <c r="A98" t="s">
         <v>491</v>
       </c>
@@ -4508,11 +5472,17 @@
       <c r="D98" s="1" t="s">
         <v>228</v>
       </c>
-      <c r="E98" s="1">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="99" spans="1:5" ht="17" x14ac:dyDescent="0.2">
+      <c r="E98" s="2" t="s">
+        <v>711</v>
+      </c>
+      <c r="F98" s="2" t="s">
+        <v>782</v>
+      </c>
+      <c r="G98" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="99" spans="1:7" ht="17" x14ac:dyDescent="0.2">
       <c r="A99" t="s">
         <v>494</v>
       </c>
@@ -4525,11 +5495,17 @@
       <c r="D99" s="1" t="s">
         <v>229</v>
       </c>
-      <c r="E99" s="1">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="100" spans="1:5" ht="17" x14ac:dyDescent="0.2">
+      <c r="E99" s="2" t="s">
+        <v>711</v>
+      </c>
+      <c r="F99" s="2" t="s">
+        <v>783</v>
+      </c>
+      <c r="G99" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="100" spans="1:7" ht="17" x14ac:dyDescent="0.2">
       <c r="A100" t="s">
         <v>497</v>
       </c>
@@ -4542,11 +5518,17 @@
       <c r="D100" s="1" t="s">
         <v>230</v>
       </c>
-      <c r="E100" s="1">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="101" spans="1:5" ht="17" x14ac:dyDescent="0.2">
+      <c r="E100" s="2" t="s">
+        <v>711</v>
+      </c>
+      <c r="F100" s="2" t="s">
+        <v>784</v>
+      </c>
+      <c r="G100" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="101" spans="1:7" ht="17" x14ac:dyDescent="0.2">
       <c r="A101" t="s">
         <v>500</v>
       </c>
@@ -4559,11 +5541,17 @@
       <c r="D101" s="1" t="s">
         <v>231</v>
       </c>
-      <c r="E101" s="1">
+      <c r="E101" s="2" t="s">
+        <v>711</v>
+      </c>
+      <c r="F101" s="2" t="s">
+        <v>785</v>
+      </c>
+      <c r="G101" s="1">
         <v>1</v>
       </c>
     </row>
-    <row r="102" spans="1:5" ht="17" x14ac:dyDescent="0.2">
+    <row r="102" spans="1:7" ht="17" x14ac:dyDescent="0.2">
       <c r="A102" t="s">
         <v>503</v>
       </c>
@@ -4576,11 +5564,17 @@
       <c r="D102" s="1" t="s">
         <v>232</v>
       </c>
-      <c r="E102" s="1">
+      <c r="E102" s="2" t="s">
+        <v>713</v>
+      </c>
+      <c r="F102" s="2" t="s">
+        <v>786</v>
+      </c>
+      <c r="G102" s="1">
         <v>0.2</v>
       </c>
     </row>
-    <row r="103" spans="1:5" ht="17" x14ac:dyDescent="0.2">
+    <row r="103" spans="1:7" ht="17" x14ac:dyDescent="0.2">
       <c r="A103" t="s">
         <v>506</v>
       </c>
@@ -4593,11 +5587,17 @@
       <c r="D103" s="1" t="s">
         <v>233</v>
       </c>
-      <c r="E103" s="1">
+      <c r="E103" s="2" t="s">
+        <v>713</v>
+      </c>
+      <c r="F103" s="2" t="s">
+        <v>787</v>
+      </c>
+      <c r="G103" s="1">
         <v>0.5</v>
       </c>
     </row>
-    <row r="104" spans="1:5" ht="17" x14ac:dyDescent="0.2">
+    <row r="104" spans="1:7" ht="17" x14ac:dyDescent="0.2">
       <c r="A104" t="s">
         <v>509</v>
       </c>
@@ -4610,11 +5610,17 @@
       <c r="D104" s="1" t="s">
         <v>234</v>
       </c>
-      <c r="E104" s="1">
+      <c r="E104" s="2" t="s">
+        <v>713</v>
+      </c>
+      <c r="F104" s="2" t="s">
+        <v>788</v>
+      </c>
+      <c r="G104" s="1">
         <v>1.2</v>
       </c>
     </row>
-    <row r="105" spans="1:5" ht="17" x14ac:dyDescent="0.2">
+    <row r="105" spans="1:7" ht="17" x14ac:dyDescent="0.2">
       <c r="A105" t="s">
         <v>512</v>
       </c>
@@ -4627,11 +5633,17 @@
       <c r="D105" s="1" t="s">
         <v>235</v>
       </c>
-      <c r="E105" s="1">
+      <c r="E105" s="2" t="s">
+        <v>713</v>
+      </c>
+      <c r="F105" s="2" t="s">
+        <v>789</v>
+      </c>
+      <c r="G105" s="1">
         <v>1.5</v>
       </c>
     </row>
-    <row r="106" spans="1:5" ht="17" x14ac:dyDescent="0.2">
+    <row r="106" spans="1:7" ht="17" x14ac:dyDescent="0.2">
       <c r="A106" t="s">
         <v>515</v>
       </c>
@@ -4644,11 +5656,17 @@
       <c r="D106" s="1" t="s">
         <v>236</v>
       </c>
-      <c r="E106" s="1">
+      <c r="E106" s="2" t="s">
+        <v>713</v>
+      </c>
+      <c r="F106" s="2" t="s">
+        <v>790</v>
+      </c>
+      <c r="G106" s="1">
         <v>2</v>
       </c>
     </row>
-    <row r="107" spans="1:5" ht="17" x14ac:dyDescent="0.2">
+    <row r="107" spans="1:7" ht="17" x14ac:dyDescent="0.2">
       <c r="A107" t="s">
         <v>518</v>
       </c>
@@ -4661,11 +5679,17 @@
       <c r="D107" s="1" t="s">
         <v>237</v>
       </c>
-      <c r="E107" s="1">
+      <c r="E107" s="2" t="s">
+        <v>713</v>
+      </c>
+      <c r="F107" s="2" t="s">
+        <v>791</v>
+      </c>
+      <c r="G107" s="1">
         <v>2.46</v>
       </c>
     </row>
-    <row r="108" spans="1:5" ht="17" x14ac:dyDescent="0.2">
+    <row r="108" spans="1:7" ht="17" x14ac:dyDescent="0.2">
       <c r="A108" t="s">
         <v>521</v>
       </c>
@@ -4678,11 +5702,17 @@
       <c r="D108" s="1" t="s">
         <v>238</v>
       </c>
-      <c r="E108" s="1">
+      <c r="E108" s="2" t="s">
+        <v>713</v>
+      </c>
+      <c r="F108" s="2" t="s">
+        <v>786</v>
+      </c>
+      <c r="G108" s="1">
         <v>2.92</v>
       </c>
     </row>
-    <row r="109" spans="1:5" ht="17" x14ac:dyDescent="0.2">
+    <row r="109" spans="1:7" ht="17" x14ac:dyDescent="0.2">
       <c r="A109" t="s">
         <v>524</v>
       </c>
@@ -4695,11 +5725,17 @@
       <c r="D109" s="1" t="s">
         <v>239</v>
       </c>
-      <c r="E109" s="1">
+      <c r="E109" s="2" t="s">
+        <v>713</v>
+      </c>
+      <c r="F109" s="2" t="s">
+        <v>787</v>
+      </c>
+      <c r="G109" s="1">
         <v>3.38</v>
       </c>
     </row>
-    <row r="110" spans="1:5" ht="17" x14ac:dyDescent="0.2">
+    <row r="110" spans="1:7" ht="17" x14ac:dyDescent="0.2">
       <c r="A110" t="s">
         <v>527</v>
       </c>
@@ -4712,11 +5748,17 @@
       <c r="D110" s="1" t="s">
         <v>240</v>
       </c>
-      <c r="E110" s="1">
+      <c r="E110" s="2" t="s">
+        <v>713</v>
+      </c>
+      <c r="F110" s="2" t="s">
+        <v>788</v>
+      </c>
+      <c r="G110" s="1">
         <v>3.84</v>
       </c>
     </row>
-    <row r="111" spans="1:5" ht="17" x14ac:dyDescent="0.2">
+    <row r="111" spans="1:7" ht="17" x14ac:dyDescent="0.2">
       <c r="A111" t="s">
         <v>530</v>
       </c>
@@ -4729,11 +5771,17 @@
       <c r="D111" s="1" t="s">
         <v>241</v>
       </c>
-      <c r="E111" s="1">
+      <c r="E111" s="2" t="s">
+        <v>713</v>
+      </c>
+      <c r="F111" s="2" t="s">
+        <v>789</v>
+      </c>
+      <c r="G111" s="1">
         <v>4.3</v>
       </c>
     </row>
-    <row r="112" spans="1:5" ht="17" x14ac:dyDescent="0.2">
+    <row r="112" spans="1:7" ht="17" x14ac:dyDescent="0.2">
       <c r="A112" t="s">
         <v>533</v>
       </c>
@@ -4746,11 +5794,17 @@
       <c r="D112" s="1" t="s">
         <v>242</v>
       </c>
-      <c r="E112" s="1">
+      <c r="E112" s="2" t="s">
+        <v>713</v>
+      </c>
+      <c r="F112" s="2" t="s">
+        <v>790</v>
+      </c>
+      <c r="G112" s="1">
         <v>4.76</v>
       </c>
     </row>
-    <row r="113" spans="1:5" ht="17" x14ac:dyDescent="0.2">
+    <row r="113" spans="1:7" ht="17" x14ac:dyDescent="0.2">
       <c r="A113" t="s">
         <v>536</v>
       </c>
@@ -4763,11 +5817,17 @@
       <c r="D113" s="1" t="s">
         <v>243</v>
       </c>
-      <c r="E113" s="1">
+      <c r="E113" s="2" t="s">
+        <v>713</v>
+      </c>
+      <c r="F113" s="2" t="s">
+        <v>791</v>
+      </c>
+      <c r="G113" s="1">
         <v>5.22</v>
       </c>
     </row>
-    <row r="114" spans="1:5" ht="17" x14ac:dyDescent="0.2">
+    <row r="114" spans="1:7" ht="17" x14ac:dyDescent="0.2">
       <c r="A114" t="s">
         <v>539</v>
       </c>
@@ -4780,11 +5840,17 @@
       <c r="D114" s="1" t="s">
         <v>244</v>
       </c>
-      <c r="E114" s="1">
+      <c r="E114" s="2" t="s">
+        <v>713</v>
+      </c>
+      <c r="F114" s="2" t="s">
+        <v>786</v>
+      </c>
+      <c r="G114" s="1">
         <v>5.68</v>
       </c>
     </row>
-    <row r="115" spans="1:5" ht="17" x14ac:dyDescent="0.2">
+    <row r="115" spans="1:7" ht="17" x14ac:dyDescent="0.2">
       <c r="A115" t="s">
         <v>542</v>
       </c>
@@ -4797,11 +5863,17 @@
       <c r="D115" s="1" t="s">
         <v>245</v>
       </c>
-      <c r="E115" s="1">
+      <c r="E115" s="2" t="s">
+        <v>713</v>
+      </c>
+      <c r="F115" s="2" t="s">
+        <v>787</v>
+      </c>
+      <c r="G115" s="1">
         <v>6.14</v>
       </c>
     </row>
-    <row r="116" spans="1:5" ht="17" x14ac:dyDescent="0.2">
+    <row r="116" spans="1:7" ht="17" x14ac:dyDescent="0.2">
       <c r="A116" t="s">
         <v>545</v>
       </c>
@@ -4814,11 +5886,17 @@
       <c r="D116" s="1" t="s">
         <v>246</v>
       </c>
-      <c r="E116" s="1">
+      <c r="E116" s="2" t="s">
+        <v>713</v>
+      </c>
+      <c r="F116" s="2" t="s">
+        <v>788</v>
+      </c>
+      <c r="G116" s="1">
         <v>6.6</v>
       </c>
     </row>
-    <row r="117" spans="1:5" ht="17" x14ac:dyDescent="0.2">
+    <row r="117" spans="1:7" ht="17" x14ac:dyDescent="0.2">
       <c r="A117" t="s">
         <v>548</v>
       </c>
@@ -4831,11 +5909,17 @@
       <c r="D117" s="1" t="s">
         <v>247</v>
       </c>
-      <c r="E117" s="1">
+      <c r="E117" s="2" t="s">
+        <v>713</v>
+      </c>
+      <c r="F117" s="2" t="s">
+        <v>789</v>
+      </c>
+      <c r="G117" s="1">
         <v>7.06</v>
       </c>
     </row>
-    <row r="118" spans="1:5" ht="17" x14ac:dyDescent="0.2">
+    <row r="118" spans="1:7" ht="17" x14ac:dyDescent="0.2">
       <c r="A118" t="s">
         <v>551</v>
       </c>
@@ -4848,11 +5932,17 @@
       <c r="D118" s="1" t="s">
         <v>248</v>
       </c>
-      <c r="E118" s="1">
+      <c r="E118" s="2" t="s">
+        <v>713</v>
+      </c>
+      <c r="F118" s="2" t="s">
+        <v>790</v>
+      </c>
+      <c r="G118" s="1">
         <v>7.52</v>
       </c>
     </row>
-    <row r="119" spans="1:5" ht="17" x14ac:dyDescent="0.2">
+    <row r="119" spans="1:7" ht="17" x14ac:dyDescent="0.2">
       <c r="A119" t="s">
         <v>554</v>
       </c>
@@ -4865,11 +5955,17 @@
       <c r="D119" s="1" t="s">
         <v>249</v>
       </c>
-      <c r="E119" s="1">
+      <c r="E119" s="2" t="s">
+        <v>713</v>
+      </c>
+      <c r="F119" s="2" t="s">
+        <v>791</v>
+      </c>
+      <c r="G119" s="1">
         <v>7.98</v>
       </c>
     </row>
-    <row r="120" spans="1:5" ht="17" x14ac:dyDescent="0.2">
+    <row r="120" spans="1:7" ht="17" x14ac:dyDescent="0.2">
       <c r="A120" t="s">
         <v>557</v>
       </c>
@@ -4882,11 +5978,17 @@
       <c r="D120" s="1" t="s">
         <v>250</v>
       </c>
-      <c r="E120" s="1">
+      <c r="E120" s="2" t="s">
+        <v>713</v>
+      </c>
+      <c r="F120" s="2" t="s">
+        <v>786</v>
+      </c>
+      <c r="G120" s="1">
         <v>8.44</v>
       </c>
     </row>
-    <row r="121" spans="1:5" ht="17" x14ac:dyDescent="0.2">
+    <row r="121" spans="1:7" ht="17" x14ac:dyDescent="0.2">
       <c r="A121" t="s">
         <v>560</v>
       </c>
@@ -4899,11 +6001,17 @@
       <c r="D121" s="1" t="s">
         <v>251</v>
       </c>
-      <c r="E121" s="1">
+      <c r="E121" s="2" t="s">
+        <v>713</v>
+      </c>
+      <c r="F121" s="2" t="s">
+        <v>787</v>
+      </c>
+      <c r="G121" s="1">
         <v>8.9</v>
       </c>
     </row>
-    <row r="122" spans="1:5" ht="17" x14ac:dyDescent="0.2">
+    <row r="122" spans="1:7" ht="17" x14ac:dyDescent="0.2">
       <c r="A122" t="s">
         <v>563</v>
       </c>
@@ -4916,11 +6024,17 @@
       <c r="D122" s="1" t="s">
         <v>252</v>
       </c>
-      <c r="E122" s="1">
+      <c r="E122" s="2" t="s">
+        <v>713</v>
+      </c>
+      <c r="F122" s="2" t="s">
+        <v>788</v>
+      </c>
+      <c r="G122" s="1">
         <v>9.36</v>
       </c>
     </row>
-    <row r="123" spans="1:5" ht="17" x14ac:dyDescent="0.2">
+    <row r="123" spans="1:7" ht="17" x14ac:dyDescent="0.2">
       <c r="A123" t="s">
         <v>566</v>
       </c>
@@ -4933,11 +6047,17 @@
       <c r="D123" s="1" t="s">
         <v>253</v>
       </c>
-      <c r="E123" s="1">
+      <c r="E123" s="2" t="s">
+        <v>713</v>
+      </c>
+      <c r="F123" s="2" t="s">
+        <v>789</v>
+      </c>
+      <c r="G123" s="1">
         <v>9.82</v>
       </c>
     </row>
-    <row r="124" spans="1:5" ht="17" x14ac:dyDescent="0.2">
+    <row r="124" spans="1:7" ht="17" x14ac:dyDescent="0.2">
       <c r="A124" t="s">
         <v>569</v>
       </c>
@@ -4950,11 +6070,17 @@
       <c r="D124" s="1" t="s">
         <v>254</v>
       </c>
-      <c r="E124" s="1">
+      <c r="E124" s="2" t="s">
+        <v>713</v>
+      </c>
+      <c r="F124" s="2" t="s">
+        <v>790</v>
+      </c>
+      <c r="G124" s="1">
         <v>2.46</v>
       </c>
     </row>
-    <row r="125" spans="1:5" ht="17" x14ac:dyDescent="0.2">
+    <row r="125" spans="1:7" ht="17" x14ac:dyDescent="0.2">
       <c r="A125" t="s">
         <v>572</v>
       </c>
@@ -4967,11 +6093,17 @@
       <c r="D125" s="1" t="s">
         <v>255</v>
       </c>
-      <c r="E125" s="1">
+      <c r="E125" s="2" t="s">
+        <v>713</v>
+      </c>
+      <c r="F125" s="2" t="s">
+        <v>791</v>
+      </c>
+      <c r="G125" s="1">
         <v>2.92</v>
       </c>
     </row>
-    <row r="126" spans="1:5" ht="17" x14ac:dyDescent="0.2">
+    <row r="126" spans="1:7" ht="17" x14ac:dyDescent="0.2">
       <c r="A126" t="s">
         <v>575</v>
       </c>
@@ -4984,11 +6116,17 @@
       <c r="D126" s="1" t="s">
         <v>256</v>
       </c>
-      <c r="E126" s="1">
+      <c r="E126" s="2" t="s">
+        <v>713</v>
+      </c>
+      <c r="F126" s="2" t="s">
+        <v>786</v>
+      </c>
+      <c r="G126" s="1">
         <v>3.38</v>
       </c>
     </row>
-    <row r="127" spans="1:5" ht="17" x14ac:dyDescent="0.2">
+    <row r="127" spans="1:7" ht="17" x14ac:dyDescent="0.2">
       <c r="A127" t="s">
         <v>578</v>
       </c>
@@ -5001,11 +6139,17 @@
       <c r="D127" s="1" t="s">
         <v>257</v>
       </c>
-      <c r="E127" s="1">
+      <c r="E127" s="2" t="s">
+        <v>713</v>
+      </c>
+      <c r="F127" s="2" t="s">
+        <v>787</v>
+      </c>
+      <c r="G127" s="1">
         <v>3.84</v>
       </c>
     </row>
-    <row r="128" spans="1:5" ht="17" x14ac:dyDescent="0.2">
+    <row r="128" spans="1:7" ht="17" x14ac:dyDescent="0.2">
       <c r="A128" t="s">
         <v>581</v>
       </c>
@@ -5018,11 +6162,17 @@
       <c r="D128" s="1" t="s">
         <v>258</v>
       </c>
-      <c r="E128" s="1">
+      <c r="E128" s="2" t="s">
+        <v>713</v>
+      </c>
+      <c r="F128" s="2" t="s">
+        <v>788</v>
+      </c>
+      <c r="G128" s="1">
         <v>4.3</v>
       </c>
     </row>
-    <row r="129" spans="1:5" ht="17" x14ac:dyDescent="0.2">
+    <row r="129" spans="1:7" ht="17" x14ac:dyDescent="0.2">
       <c r="A129" t="s">
         <v>584</v>
       </c>
@@ -5035,11 +6185,17 @@
       <c r="D129" s="1" t="s">
         <v>259</v>
       </c>
-      <c r="E129" s="1">
+      <c r="E129" s="2" t="s">
+        <v>713</v>
+      </c>
+      <c r="F129" s="2" t="s">
+        <v>789</v>
+      </c>
+      <c r="G129" s="1">
         <v>4.76</v>
       </c>
     </row>
-    <row r="130" spans="1:5" ht="17" x14ac:dyDescent="0.2">
+    <row r="130" spans="1:7" ht="17" x14ac:dyDescent="0.2">
       <c r="A130" t="s">
         <v>587</v>
       </c>
@@ -5052,11 +6208,17 @@
       <c r="D130" s="1" t="s">
         <v>260</v>
       </c>
-      <c r="E130" s="1">
+      <c r="E130" s="2" t="s">
+        <v>713</v>
+      </c>
+      <c r="F130" s="2" t="s">
+        <v>790</v>
+      </c>
+      <c r="G130" s="1">
         <v>5.22</v>
       </c>
     </row>
-    <row r="131" spans="1:5" ht="17" x14ac:dyDescent="0.2">
+    <row r="131" spans="1:7" ht="17" x14ac:dyDescent="0.2">
       <c r="A131" t="s">
         <v>590</v>
       </c>
@@ -5069,11 +6231,17 @@
       <c r="D131" s="1" t="s">
         <v>261</v>
       </c>
-      <c r="E131" s="1">
+      <c r="E131" s="2" t="s">
+        <v>713</v>
+      </c>
+      <c r="F131" s="2" t="s">
+        <v>791</v>
+      </c>
+      <c r="G131" s="1">
         <v>5.68</v>
       </c>
     </row>
-    <row r="132" spans="1:5" ht="17" x14ac:dyDescent="0.2">
+    <row r="132" spans="1:7" ht="17" x14ac:dyDescent="0.2">
       <c r="A132" t="s">
         <v>593</v>
       </c>
@@ -5086,11 +6254,17 @@
       <c r="D132" s="1" t="s">
         <v>262</v>
       </c>
-      <c r="E132" s="1">
+      <c r="E132" s="2" t="s">
+        <v>713</v>
+      </c>
+      <c r="F132" s="2" t="s">
+        <v>786</v>
+      </c>
+      <c r="G132" s="1">
         <v>6.14</v>
       </c>
     </row>
-    <row r="133" spans="1:5" ht="17" x14ac:dyDescent="0.2">
+    <row r="133" spans="1:7" ht="17" x14ac:dyDescent="0.2">
       <c r="A133" t="s">
         <v>596</v>
       </c>
@@ -5103,11 +6277,17 @@
       <c r="D133" s="1" t="s">
         <v>263</v>
       </c>
-      <c r="E133" s="1">
+      <c r="E133" s="2" t="s">
+        <v>713</v>
+      </c>
+      <c r="F133" s="2" t="s">
+        <v>787</v>
+      </c>
+      <c r="G133" s="1">
         <v>6.6</v>
       </c>
     </row>
-    <row r="134" spans="1:5" ht="17" x14ac:dyDescent="0.2">
+    <row r="134" spans="1:7" ht="17" x14ac:dyDescent="0.2">
       <c r="A134" t="s">
         <v>599</v>
       </c>
@@ -5120,11 +6300,17 @@
       <c r="D134" s="1" t="s">
         <v>264</v>
       </c>
-      <c r="E134" s="1">
+      <c r="E134" s="2" t="s">
+        <v>713</v>
+      </c>
+      <c r="F134" s="2" t="s">
+        <v>788</v>
+      </c>
+      <c r="G134" s="1">
         <v>7.06</v>
       </c>
     </row>
-    <row r="135" spans="1:5" ht="17" x14ac:dyDescent="0.2">
+    <row r="135" spans="1:7" ht="17" x14ac:dyDescent="0.2">
       <c r="A135" t="s">
         <v>602</v>
       </c>
@@ -5137,11 +6323,17 @@
       <c r="D135" s="1" t="s">
         <v>265</v>
       </c>
-      <c r="E135" s="1">
+      <c r="E135" s="2" t="s">
+        <v>713</v>
+      </c>
+      <c r="F135" s="2" t="s">
+        <v>789</v>
+      </c>
+      <c r="G135" s="1">
         <v>7.52</v>
       </c>
     </row>
-    <row r="136" spans="1:5" ht="17" x14ac:dyDescent="0.2">
+    <row r="136" spans="1:7" ht="17" x14ac:dyDescent="0.2">
       <c r="A136" t="s">
         <v>605</v>
       </c>
@@ -5154,11 +6346,17 @@
       <c r="D136" s="1" t="s">
         <v>266</v>
       </c>
-      <c r="E136" s="1">
+      <c r="E136" s="2" t="s">
+        <v>713</v>
+      </c>
+      <c r="F136" s="2" t="s">
+        <v>790</v>
+      </c>
+      <c r="G136" s="1">
         <v>7.98</v>
       </c>
     </row>
-    <row r="137" spans="1:5" ht="17" x14ac:dyDescent="0.2">
+    <row r="137" spans="1:7" ht="17" x14ac:dyDescent="0.2">
       <c r="A137" t="s">
         <v>608</v>
       </c>
@@ -5171,11 +6369,17 @@
       <c r="D137" s="1" t="s">
         <v>267</v>
       </c>
-      <c r="E137" s="1">
+      <c r="E137" s="2" t="s">
+        <v>713</v>
+      </c>
+      <c r="F137" s="2" t="s">
+        <v>791</v>
+      </c>
+      <c r="G137" s="1">
         <v>8.44</v>
       </c>
     </row>
-    <row r="138" spans="1:5" ht="17" x14ac:dyDescent="0.2">
+    <row r="138" spans="1:7" ht="17" x14ac:dyDescent="0.2">
       <c r="A138" t="s">
         <v>611</v>
       </c>
@@ -5188,11 +6392,17 @@
       <c r="D138" s="1" t="s">
         <v>268</v>
       </c>
-      <c r="E138" s="1">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="139" spans="1:5" ht="17" x14ac:dyDescent="0.2">
+      <c r="E138" s="2" t="s">
+        <v>711</v>
+      </c>
+      <c r="F138" s="2" t="s">
+        <v>792</v>
+      </c>
+      <c r="G138" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="139" spans="1:7" ht="17" x14ac:dyDescent="0.2">
       <c r="A139" t="s">
         <v>614</v>
       </c>
@@ -5205,11 +6415,17 @@
       <c r="D139" s="1" t="s">
         <v>269</v>
       </c>
-      <c r="E139" s="1">
+      <c r="E139" s="2" t="s">
+        <v>711</v>
+      </c>
+      <c r="F139" s="2" t="s">
+        <v>793</v>
+      </c>
+      <c r="G139" s="1">
         <v>1</v>
       </c>
     </row>
-    <row r="140" spans="1:5" ht="17" x14ac:dyDescent="0.2">
+    <row r="140" spans="1:7" ht="17" x14ac:dyDescent="0.2">
       <c r="A140" t="s">
         <v>617</v>
       </c>
@@ -5222,11 +6438,17 @@
       <c r="D140" s="1" t="s">
         <v>270</v>
       </c>
-      <c r="E140" s="1">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="141" spans="1:5" ht="17" x14ac:dyDescent="0.2">
+      <c r="E140" s="2" t="s">
+        <v>711</v>
+      </c>
+      <c r="F140" s="2" t="s">
+        <v>794</v>
+      </c>
+      <c r="G140" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="141" spans="1:7" ht="17" x14ac:dyDescent="0.2">
       <c r="A141" t="s">
         <v>620</v>
       </c>
@@ -5239,11 +6461,17 @@
       <c r="D141" s="1" t="s">
         <v>271</v>
       </c>
-      <c r="E141" s="1">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="142" spans="1:5" ht="17" x14ac:dyDescent="0.2">
+      <c r="E141" s="2" t="s">
+        <v>711</v>
+      </c>
+      <c r="F141" s="2" t="s">
+        <v>795</v>
+      </c>
+      <c r="G141" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="142" spans="1:7" ht="17" x14ac:dyDescent="0.2">
       <c r="A142" t="s">
         <v>623</v>
       </c>
@@ -5256,11 +6484,17 @@
       <c r="D142" s="1" t="s">
         <v>272</v>
       </c>
-      <c r="E142" s="1">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="143" spans="1:5" ht="17" x14ac:dyDescent="0.2">
+      <c r="E142" s="2" t="s">
+        <v>711</v>
+      </c>
+      <c r="F142" s="2" t="s">
+        <v>740</v>
+      </c>
+      <c r="G142" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="143" spans="1:7" ht="17" x14ac:dyDescent="0.2">
       <c r="A143" t="s">
         <v>626</v>
       </c>
@@ -5273,11 +6507,17 @@
       <c r="D143" s="1" t="s">
         <v>273</v>
       </c>
-      <c r="E143" s="1">
+      <c r="E143" s="2" t="s">
+        <v>711</v>
+      </c>
+      <c r="F143" s="2" t="s">
+        <v>741</v>
+      </c>
+      <c r="G143" s="1">
         <v>1</v>
       </c>
     </row>
-    <row r="144" spans="1:5" ht="17" x14ac:dyDescent="0.2">
+    <row r="144" spans="1:7" ht="17" x14ac:dyDescent="0.2">
       <c r="A144" t="s">
         <v>629</v>
       </c>
@@ -5290,11 +6530,17 @@
       <c r="D144" s="1" t="s">
         <v>274</v>
       </c>
-      <c r="E144" s="1">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="145" spans="1:5" ht="17" x14ac:dyDescent="0.2">
+      <c r="E144" s="2" t="s">
+        <v>711</v>
+      </c>
+      <c r="F144" s="2" t="s">
+        <v>796</v>
+      </c>
+      <c r="G144" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="145" spans="1:7" ht="17" x14ac:dyDescent="0.2">
       <c r="A145" t="s">
         <v>632</v>
       </c>
@@ -5307,11 +6553,17 @@
       <c r="D145" s="1" t="s">
         <v>275</v>
       </c>
-      <c r="E145" s="1">
+      <c r="E145" s="2" t="s">
+        <v>711</v>
+      </c>
+      <c r="F145" s="2" t="s">
+        <v>797</v>
+      </c>
+      <c r="G145" s="1">
         <v>1</v>
       </c>
     </row>
-    <row r="146" spans="1:5" ht="17" x14ac:dyDescent="0.2">
+    <row r="146" spans="1:7" ht="17" x14ac:dyDescent="0.2">
       <c r="A146" t="s">
         <v>635</v>
       </c>
@@ -5324,11 +6576,17 @@
       <c r="D146" s="1" t="s">
         <v>276</v>
       </c>
-      <c r="E146" s="1">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="147" spans="1:5" ht="17" x14ac:dyDescent="0.2">
+      <c r="E146" s="2" t="s">
+        <v>711</v>
+      </c>
+      <c r="F146" s="2" t="s">
+        <v>798</v>
+      </c>
+      <c r="G146" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="147" spans="1:7" ht="17" x14ac:dyDescent="0.2">
       <c r="A147" t="s">
         <v>638</v>
       </c>
@@ -5341,11 +6599,17 @@
       <c r="D147" s="1" t="s">
         <v>277</v>
       </c>
-      <c r="E147" s="1">
+      <c r="E147" s="2" t="s">
+        <v>711</v>
+      </c>
+      <c r="F147" s="2" t="s">
+        <v>799</v>
+      </c>
+      <c r="G147" s="1">
         <v>1</v>
       </c>
     </row>
-    <row r="148" spans="1:5" ht="17" x14ac:dyDescent="0.2">
+    <row r="148" spans="1:7" ht="17" x14ac:dyDescent="0.2">
       <c r="A148" t="s">
         <v>641</v>
       </c>
@@ -5358,11 +6622,17 @@
       <c r="D148" s="1" t="s">
         <v>278</v>
       </c>
-      <c r="E148" s="1">
+      <c r="E148" s="2" t="s">
+        <v>711</v>
+      </c>
+      <c r="F148" s="2" t="s">
+        <v>800</v>
+      </c>
+      <c r="G148" s="1">
         <v>1</v>
       </c>
     </row>
-    <row r="149" spans="1:5" ht="17" x14ac:dyDescent="0.2">
+    <row r="149" spans="1:7" ht="17" x14ac:dyDescent="0.2">
       <c r="A149" t="s">
         <v>644</v>
       </c>
@@ -5375,11 +6645,17 @@
       <c r="D149" s="1" t="s">
         <v>279</v>
       </c>
-      <c r="E149" s="1">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="150" spans="1:5" ht="17" x14ac:dyDescent="0.2">
+      <c r="E149" s="2" t="s">
+        <v>711</v>
+      </c>
+      <c r="F149" s="2" t="s">
+        <v>801</v>
+      </c>
+      <c r="G149" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="150" spans="1:7" ht="17" x14ac:dyDescent="0.2">
       <c r="A150" t="s">
         <v>647</v>
       </c>
@@ -5392,11 +6668,17 @@
       <c r="D150" s="1" t="s">
         <v>280</v>
       </c>
-      <c r="E150" s="1">
+      <c r="E150" s="2" t="s">
+        <v>711</v>
+      </c>
+      <c r="F150" s="2" t="s">
+        <v>802</v>
+      </c>
+      <c r="G150" s="1">
         <v>1</v>
       </c>
     </row>
-    <row r="151" spans="1:5" ht="17" x14ac:dyDescent="0.2">
+    <row r="151" spans="1:7" ht="17" x14ac:dyDescent="0.2">
       <c r="A151" t="s">
         <v>650</v>
       </c>
@@ -5409,11 +6691,17 @@
       <c r="D151" s="1" t="s">
         <v>281</v>
       </c>
-      <c r="E151" s="1">
+      <c r="E151" s="2" t="s">
+        <v>711</v>
+      </c>
+      <c r="F151" s="2" t="s">
+        <v>803</v>
+      </c>
+      <c r="G151" s="1">
         <v>1</v>
       </c>
     </row>
-    <row r="152" spans="1:5" ht="17" x14ac:dyDescent="0.2">
+    <row r="152" spans="1:7" ht="17" x14ac:dyDescent="0.2">
       <c r="A152" t="s">
         <v>653</v>
       </c>
@@ -5426,11 +6714,17 @@
       <c r="D152" s="1" t="s">
         <v>282</v>
       </c>
-      <c r="E152" s="1">
+      <c r="E152" s="2" t="s">
+        <v>711</v>
+      </c>
+      <c r="F152" s="2" t="s">
+        <v>800</v>
+      </c>
+      <c r="G152" s="1">
         <v>1</v>
       </c>
     </row>
-    <row r="153" spans="1:5" ht="17" x14ac:dyDescent="0.2">
+    <row r="153" spans="1:7" ht="17" x14ac:dyDescent="0.2">
       <c r="A153" t="s">
         <v>656</v>
       </c>
@@ -5443,11 +6737,17 @@
       <c r="D153" s="1" t="s">
         <v>283</v>
       </c>
-      <c r="E153" s="1">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="154" spans="1:5" ht="17" x14ac:dyDescent="0.2">
+      <c r="E153" s="2" t="s">
+        <v>711</v>
+      </c>
+      <c r="F153" s="2" t="s">
+        <v>801</v>
+      </c>
+      <c r="G153" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="154" spans="1:7" ht="17" x14ac:dyDescent="0.2">
       <c r="A154" t="s">
         <v>659</v>
       </c>
@@ -5460,11 +6760,17 @@
       <c r="D154" s="1" t="s">
         <v>284</v>
       </c>
-      <c r="E154" s="1">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="155" spans="1:5" ht="17" x14ac:dyDescent="0.2">
+      <c r="E154" s="2" t="s">
+        <v>711</v>
+      </c>
+      <c r="F154" s="2" t="s">
+        <v>802</v>
+      </c>
+      <c r="G154" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="155" spans="1:7" ht="17" x14ac:dyDescent="0.2">
       <c r="A155" t="s">
         <v>662</v>
       </c>
@@ -5477,11 +6783,17 @@
       <c r="D155" s="1" t="s">
         <v>285</v>
       </c>
-      <c r="E155" s="1">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="156" spans="1:5" ht="17" x14ac:dyDescent="0.2">
+      <c r="E155" s="2" t="s">
+        <v>711</v>
+      </c>
+      <c r="F155" s="2" t="s">
+        <v>803</v>
+      </c>
+      <c r="G155" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="156" spans="1:7" ht="17" x14ac:dyDescent="0.2">
       <c r="A156" t="s">
         <v>665</v>
       </c>
@@ -5494,11 +6806,17 @@
       <c r="D156" s="1" t="s">
         <v>286</v>
       </c>
-      <c r="E156" s="1">
+      <c r="E156" s="2" t="s">
+        <v>711</v>
+      </c>
+      <c r="F156" s="2" t="s">
+        <v>804</v>
+      </c>
+      <c r="G156" s="1">
         <v>1</v>
       </c>
     </row>
-    <row r="157" spans="1:5" ht="17" x14ac:dyDescent="0.2">
+    <row r="157" spans="1:7" ht="17" x14ac:dyDescent="0.2">
       <c r="A157" t="s">
         <v>668</v>
       </c>
@@ -5511,11 +6829,17 @@
       <c r="D157" s="1" t="s">
         <v>287</v>
       </c>
-      <c r="E157" s="1">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="158" spans="1:5" ht="17" x14ac:dyDescent="0.2">
+      <c r="E157" s="2" t="s">
+        <v>711</v>
+      </c>
+      <c r="F157" s="2" t="s">
+        <v>805</v>
+      </c>
+      <c r="G157" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="158" spans="1:7" ht="17" x14ac:dyDescent="0.2">
       <c r="A158" t="s">
         <v>671</v>
       </c>
@@ -5528,11 +6852,17 @@
       <c r="D158" s="1" t="s">
         <v>288</v>
       </c>
-      <c r="E158" s="1">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="159" spans="1:5" ht="17" x14ac:dyDescent="0.2">
+      <c r="E158" s="2" t="s">
+        <v>711</v>
+      </c>
+      <c r="F158" s="2" t="s">
+        <v>806</v>
+      </c>
+      <c r="G158" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="159" spans="1:7" ht="17" x14ac:dyDescent="0.2">
       <c r="A159" t="s">
         <v>674</v>
       </c>
@@ -5545,11 +6875,17 @@
       <c r="D159" s="1" t="s">
         <v>289</v>
       </c>
-      <c r="E159" s="1">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="160" spans="1:5" ht="17" x14ac:dyDescent="0.2">
+      <c r="E159" s="2" t="s">
+        <v>711</v>
+      </c>
+      <c r="F159" s="2" t="s">
+        <v>807</v>
+      </c>
+      <c r="G159" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="160" spans="1:7" ht="17" x14ac:dyDescent="0.2">
       <c r="A160" t="s">
         <v>677</v>
       </c>
@@ -5562,11 +6898,17 @@
       <c r="D160" s="1" t="s">
         <v>290</v>
       </c>
-      <c r="E160" s="1">
+      <c r="E160" s="2" t="s">
+        <v>711</v>
+      </c>
+      <c r="F160" s="2" t="s">
+        <v>808</v>
+      </c>
+      <c r="G160" s="1">
         <v>1</v>
       </c>
     </row>
-    <row r="161" spans="1:5" ht="17" x14ac:dyDescent="0.2">
+    <row r="161" spans="1:7" ht="17" x14ac:dyDescent="0.2">
       <c r="A161" t="s">
         <v>680</v>
       </c>
@@ -5579,11 +6921,17 @@
       <c r="D161" s="1" t="s">
         <v>291</v>
       </c>
-      <c r="E161" s="1">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="162" spans="1:5" ht="17" x14ac:dyDescent="0.2">
+      <c r="E161" s="2" t="s">
+        <v>711</v>
+      </c>
+      <c r="F161" s="2" t="s">
+        <v>809</v>
+      </c>
+      <c r="G161" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="162" spans="1:7" ht="17" x14ac:dyDescent="0.2">
       <c r="A162" t="s">
         <v>683</v>
       </c>
@@ -5596,7 +6944,13 @@
       <c r="D162" s="1" t="s">
         <v>292</v>
       </c>
-      <c r="E162" s="1">
+      <c r="E162" s="2" t="s">
+        <v>711</v>
+      </c>
+      <c r="F162" s="2" t="s">
+        <v>810</v>
+      </c>
+      <c r="G162" s="1">
         <v>1</v>
       </c>
     </row>
@@ -5604,7 +6958,7 @@
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <ignoredErrors>
-    <ignoredError sqref="A1:E1 A2:C2" numberStoredAsText="1"/>
+    <ignoredError sqref="G1 A2:C2 A1:D1" numberStoredAsText="1"/>
   </ignoredErrors>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
simulate realtime ohc monitoring
</commit_message>
<xml_diff>
--- a/prisma/seed/seed_data.xlsx
+++ b/prisma/seed/seed_data.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11207"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24332"/>
   <workbookPr codeName="ThisWorkbook"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/rafly/Data/Dev/Project/monitoring-welding-body/prisma/seed/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Dev\pr\monitoring-welding-body\prisma\seed\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E4B4F59B-7845-CE42-94DF-81ABF8F3A03C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E183BE2B-3D18-483F-A9A2-A3D84482BC27}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="500" windowWidth="33600" windowHeight="19100" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-103" yWindow="-103" windowWidth="24892" windowHeight="14914" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Permissions" sheetId="1" r:id="rId1"/>
@@ -19,7 +19,8 @@
     <sheet name="Users" sheetId="4" r:id="rId4"/>
     <sheet name="Assets" sheetId="5" r:id="rId5"/>
   </sheets>
-  <calcPr calcId="0"/>
+  <calcPr calcId="181029"/>
+  <fileRecoveryPr repairLoad="1"/>
 </workbook>
 </file>
 
@@ -1036,7 +1037,7 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="1">
-    <numFmt numFmtId="168" formatCode="0000"/>
+    <numFmt numFmtId="164" formatCode="0000"/>
   </numFmts>
   <fonts count="4" x14ac:knownFonts="1">
     <font>
@@ -1096,7 +1097,7 @@
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="168" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" shrinkToFit="1"/>
     </xf>
   </cellXfs>
@@ -1438,19 +1439,20 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <sheetPr codeName="Sheet1"/>
   <dimension ref="A1:B11"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="B7" sqref="B7:B11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="10.85546875" defaultRowHeight="15.9" x14ac:dyDescent="0.45"/>
   <cols>
-    <col min="1" max="1" width="13.33203125" customWidth="1"/>
+    <col min="1" max="1" width="13.35546875" customWidth="1"/>
     <col min="2" max="2" width="18.5" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -1458,7 +1460,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A2" t="s">
         <v>2</v>
       </c>
@@ -1466,7 +1468,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A3" t="s">
         <v>4</v>
       </c>
@@ -1474,7 +1476,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A4" t="s">
         <v>6</v>
       </c>
@@ -1482,7 +1484,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A5" t="s">
         <v>8</v>
       </c>
@@ -1490,7 +1492,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A6" t="s">
         <v>10</v>
       </c>
@@ -1498,7 +1500,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A7" t="s">
         <v>32</v>
       </c>
@@ -1506,7 +1508,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A8" t="s">
         <v>33</v>
       </c>
@@ -1514,7 +1516,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A9" t="s">
         <v>34</v>
       </c>
@@ -1522,7 +1524,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A10" t="s">
         <v>35</v>
       </c>
@@ -1530,7 +1532,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="11" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A11" t="s">
         <v>36</v>
       </c>
@@ -1548,19 +1550,20 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
+  <sheetPr codeName="Sheet2"/>
   <dimension ref="A1:B15"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="E15" sqref="E15"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="10.85546875" defaultRowHeight="15.9" x14ac:dyDescent="0.45"/>
   <cols>
-    <col min="1" max="1" width="10.6640625" customWidth="1"/>
-    <col min="2" max="2" width="16.83203125" customWidth="1"/>
+    <col min="1" max="1" width="10.640625" customWidth="1"/>
+    <col min="2" max="2" width="16.85546875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A1" t="s">
         <v>12</v>
       </c>
@@ -1568,7 +1571,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A2" t="s">
         <v>14</v>
       </c>
@@ -1576,7 +1579,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A3" t="s">
         <v>14</v>
       </c>
@@ -1584,7 +1587,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A4" t="s">
         <v>14</v>
       </c>
@@ -1592,7 +1595,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A5" t="s">
         <v>14</v>
       </c>
@@ -1600,7 +1603,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A6" t="s">
         <v>14</v>
       </c>
@@ -1608,7 +1611,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A7" t="s">
         <v>14</v>
       </c>
@@ -1616,7 +1619,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A8" t="s">
         <v>14</v>
       </c>
@@ -1624,7 +1627,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A9" t="s">
         <v>14</v>
       </c>
@@ -1632,7 +1635,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A10" t="s">
         <v>14</v>
       </c>
@@ -1640,7 +1643,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="11" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A11" t="s">
         <v>14</v>
       </c>
@@ -1648,7 +1651,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="12" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A12" t="s">
         <v>15</v>
       </c>
@@ -1656,7 +1659,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="13" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A13" t="s">
         <v>15</v>
       </c>
@@ -1664,7 +1667,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="14" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A14" t="s">
         <v>15</v>
       </c>
@@ -1672,7 +1675,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="15" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A15" t="s">
         <v>15</v>
       </c>
@@ -1690,13 +1693,14 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
+  <sheetPr codeName="Sheet3"/>
   <dimension ref="A1:B3"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="10.85546875" defaultRowHeight="15.9" x14ac:dyDescent="0.45"/>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A1" t="s">
         <v>16</v>
       </c>
@@ -1704,7 +1708,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A2" t="s">
         <v>17</v>
       </c>
@@ -1712,7 +1716,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A3" t="s">
         <v>18</v>
       </c>
@@ -1730,20 +1734,21 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
+  <sheetPr codeName="Sheet4"/>
   <dimension ref="A1:E3"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="10.85546875" defaultRowHeight="15.9" x14ac:dyDescent="0.45"/>
   <cols>
-    <col min="1" max="1" width="15.83203125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="25.6640625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="9.33203125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="15.85546875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="25.640625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="9.35546875" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="12" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="9" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -1760,7 +1765,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A2" t="s">
         <v>22</v>
       </c>
@@ -1777,7 +1782,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A3" t="s">
         <v>25</v>
       </c>
@@ -1804,21 +1809,22 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
+  <sheetPr codeName="Sheet5"/>
   <dimension ref="A1:G162"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A19" workbookViewId="0">
-      <selection activeCell="G12" sqref="G12"/>
+    <sheetView tabSelected="1" topLeftCell="A75" workbookViewId="0">
+      <selection activeCell="C80" sqref="C80"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="10.85546875" defaultRowHeight="15.9" x14ac:dyDescent="0.45"/>
   <cols>
-    <col min="1" max="1" width="65.83203125" bestFit="1" customWidth="1"/>
-    <col min="2" max="3" width="10.83203125" style="1"/>
-    <col min="5" max="5" width="17.33203125" customWidth="1"/>
-    <col min="6" max="6" width="41.83203125" customWidth="1"/>
+    <col min="1" max="1" width="65.85546875" bestFit="1" customWidth="1"/>
+    <col min="2" max="3" width="10.85546875" style="1"/>
+    <col min="5" max="5" width="17.35546875" customWidth="1"/>
+    <col min="6" max="6" width="41.85546875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A1" s="3" t="s">
         <v>27</v>
       </c>
@@ -1841,7 +1847,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="2" spans="1:7" ht="17" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A2" s="3" t="s">
         <v>328</v>
       </c>
@@ -1864,7 +1870,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:7" ht="17" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A3" s="3" t="s">
         <v>328</v>
       </c>
@@ -1887,7 +1893,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="4" spans="1:7" ht="17" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A4" s="3" t="s">
         <v>328</v>
       </c>
@@ -1910,7 +1916,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="5" spans="1:7" ht="17" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A5" s="3" t="s">
         <v>328</v>
       </c>
@@ -1933,7 +1939,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="6" spans="1:7" ht="17" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A6" s="3" t="s">
         <v>328</v>
       </c>
@@ -1956,7 +1962,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="7" spans="1:7" ht="17" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A7" s="3" t="s">
         <v>328</v>
       </c>
@@ -1979,7 +1985,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="8" spans="1:7" ht="17" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A8" s="3" t="s">
         <v>328</v>
       </c>
@@ -2002,7 +2008,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="9" spans="1:7" ht="17" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A9" s="3" t="s">
         <v>328</v>
       </c>
@@ -2025,7 +2031,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="10" spans="1:7" ht="17" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A10" s="3" t="s">
         <v>328</v>
       </c>
@@ -2048,7 +2054,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="11" spans="1:7" ht="17" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A11" s="3" t="s">
         <v>328</v>
       </c>
@@ -2071,7 +2077,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="12" spans="1:7" ht="17" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A12" s="3" t="s">
         <v>328</v>
       </c>
@@ -2094,7 +2100,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="13" spans="1:7" ht="17" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A13" s="3" t="s">
         <v>328</v>
       </c>
@@ -2117,7 +2123,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="14" spans="1:7" ht="17" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A14" s="3" t="s">
         <v>328</v>
       </c>
@@ -2140,7 +2146,7 @@
         <v>67</v>
       </c>
     </row>
-    <row r="15" spans="1:7" ht="17" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A15" s="3" t="s">
         <v>328</v>
       </c>
@@ -2163,7 +2169,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="16" spans="1:7" ht="17" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A16" s="3" t="s">
         <v>328</v>
       </c>
@@ -2186,7 +2192,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="17" spans="1:7" ht="17" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A17" s="3" t="s">
         <v>328</v>
       </c>
@@ -2209,7 +2215,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="18" spans="1:7" ht="17" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A18" s="3" t="s">
         <v>328</v>
       </c>
@@ -2232,7 +2238,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="19" spans="1:7" ht="17" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A19" s="3" t="s">
         <v>328</v>
       </c>
@@ -2255,7 +2261,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="20" spans="1:7" ht="17" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A20" s="3" t="s">
         <v>328</v>
       </c>
@@ -2278,7 +2284,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="21" spans="1:7" ht="17" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A21" s="3" t="s">
         <v>328</v>
       </c>
@@ -2301,7 +2307,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="22" spans="1:7" ht="17" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A22" s="3" t="s">
         <v>328</v>
       </c>
@@ -2324,7 +2330,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="23" spans="1:7" ht="17" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A23" s="3" t="s">
         <v>328</v>
       </c>
@@ -2347,7 +2353,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="24" spans="1:7" ht="17" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A24" s="3" t="s">
         <v>328</v>
       </c>
@@ -2370,7 +2376,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="25" spans="1:7" ht="17" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A25" s="3" t="s">
         <v>328</v>
       </c>
@@ -2393,7 +2399,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="26" spans="1:7" ht="17" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A26" s="3" t="s">
         <v>328</v>
       </c>
@@ -2416,7 +2422,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="27" spans="1:7" ht="17" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A27" s="3" t="s">
         <v>328</v>
       </c>
@@ -2439,7 +2445,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="28" spans="1:7" ht="17" x14ac:dyDescent="0.2">
+    <row r="28" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A28" s="3" t="s">
         <v>328</v>
       </c>
@@ -2462,7 +2468,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="29" spans="1:7" ht="17" x14ac:dyDescent="0.2">
+    <row r="29" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A29" s="3" t="s">
         <v>328</v>
       </c>
@@ -2485,7 +2491,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="30" spans="1:7" ht="17" x14ac:dyDescent="0.2">
+    <row r="30" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A30" s="3" t="s">
         <v>328</v>
       </c>
@@ -2508,7 +2514,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="31" spans="1:7" ht="17" x14ac:dyDescent="0.2">
+    <row r="31" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A31" s="3" t="s">
         <v>328</v>
       </c>
@@ -2531,7 +2537,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="32" spans="1:7" ht="17" x14ac:dyDescent="0.2">
+    <row r="32" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A32" s="3" t="s">
         <v>328</v>
       </c>
@@ -2554,7 +2560,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="33" spans="1:7" ht="17" x14ac:dyDescent="0.2">
+    <row r="33" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A33" s="3" t="s">
         <v>328</v>
       </c>
@@ -2577,7 +2583,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="34" spans="1:7" ht="17" x14ac:dyDescent="0.2">
+    <row r="34" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A34" s="3" t="s">
         <v>328</v>
       </c>
@@ -2600,7 +2606,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="35" spans="1:7" ht="17" x14ac:dyDescent="0.2">
+    <row r="35" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A35" s="3" t="s">
         <v>328</v>
       </c>
@@ -2623,7 +2629,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="36" spans="1:7" ht="17" x14ac:dyDescent="0.2">
+    <row r="36" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A36" s="3" t="s">
         <v>328</v>
       </c>
@@ -2646,7 +2652,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="37" spans="1:7" ht="17" x14ac:dyDescent="0.2">
+    <row r="37" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A37" s="3" t="s">
         <v>328</v>
       </c>
@@ -2669,7 +2675,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="38" spans="1:7" ht="17" x14ac:dyDescent="0.2">
+    <row r="38" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A38" s="3" t="s">
         <v>328</v>
       </c>
@@ -2692,7 +2698,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="39" spans="1:7" ht="17" x14ac:dyDescent="0.2">
+    <row r="39" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A39" s="3" t="s">
         <v>328</v>
       </c>
@@ -2715,7 +2721,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="40" spans="1:7" ht="17" x14ac:dyDescent="0.2">
+    <row r="40" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A40" s="3" t="s">
         <v>328</v>
       </c>
@@ -2738,7 +2744,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="41" spans="1:7" ht="17" x14ac:dyDescent="0.2">
+    <row r="41" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A41" s="3" t="s">
         <v>328</v>
       </c>
@@ -2761,7 +2767,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="42" spans="1:7" ht="17" x14ac:dyDescent="0.2">
+    <row r="42" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A42" s="3" t="s">
         <v>328</v>
       </c>
@@ -2784,7 +2790,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="43" spans="1:7" ht="17" x14ac:dyDescent="0.2">
+    <row r="43" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A43" s="3" t="s">
         <v>328</v>
       </c>
@@ -2807,7 +2813,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="44" spans="1:7" ht="17" x14ac:dyDescent="0.2">
+    <row r="44" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A44" s="3" t="s">
         <v>328</v>
       </c>
@@ -2830,7 +2836,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="45" spans="1:7" ht="17" x14ac:dyDescent="0.2">
+    <row r="45" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A45" s="3" t="s">
         <v>328</v>
       </c>
@@ -2853,7 +2859,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="46" spans="1:7" ht="17" x14ac:dyDescent="0.2">
+    <row r="46" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A46" s="3" t="s">
         <v>328</v>
       </c>
@@ -2876,7 +2882,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="47" spans="1:7" ht="17" x14ac:dyDescent="0.2">
+    <row r="47" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A47" s="3" t="s">
         <v>328</v>
       </c>
@@ -2899,7 +2905,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="48" spans="1:7" ht="17" x14ac:dyDescent="0.2">
+    <row r="48" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A48" s="3" t="s">
         <v>328</v>
       </c>
@@ -2922,7 +2928,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="49" spans="1:7" ht="17" x14ac:dyDescent="0.2">
+    <row r="49" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A49" s="3" t="s">
         <v>328</v>
       </c>
@@ -2945,7 +2951,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="50" spans="1:7" ht="17" x14ac:dyDescent="0.2">
+    <row r="50" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A50" s="3" t="s">
         <v>328</v>
       </c>
@@ -2968,7 +2974,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="51" spans="1:7" ht="17" x14ac:dyDescent="0.2">
+    <row r="51" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A51" s="3" t="s">
         <v>328</v>
       </c>
@@ -2991,7 +2997,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="52" spans="1:7" ht="17" x14ac:dyDescent="0.2">
+    <row r="52" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A52" s="3" t="s">
         <v>328</v>
       </c>
@@ -3014,7 +3020,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="53" spans="1:7" ht="17" x14ac:dyDescent="0.2">
+    <row r="53" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A53" s="3" t="s">
         <v>328</v>
       </c>
@@ -3037,7 +3043,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="54" spans="1:7" ht="17" x14ac:dyDescent="0.2">
+    <row r="54" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A54" s="3" t="s">
         <v>328</v>
       </c>
@@ -3060,7 +3066,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="55" spans="1:7" ht="17" x14ac:dyDescent="0.2">
+    <row r="55" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A55" s="3" t="s">
         <v>328</v>
       </c>
@@ -3083,7 +3089,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="56" spans="1:7" ht="17" x14ac:dyDescent="0.2">
+    <row r="56" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A56" s="3" t="s">
         <v>328</v>
       </c>
@@ -3106,7 +3112,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="57" spans="1:7" ht="17" x14ac:dyDescent="0.2">
+    <row r="57" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A57" s="3" t="s">
         <v>328</v>
       </c>
@@ -3129,7 +3135,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="58" spans="1:7" ht="17" x14ac:dyDescent="0.2">
+    <row r="58" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A58" s="3" t="s">
         <v>328</v>
       </c>
@@ -3152,7 +3158,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="59" spans="1:7" ht="17" x14ac:dyDescent="0.2">
+    <row r="59" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A59" s="3" t="s">
         <v>328</v>
       </c>
@@ -3175,7 +3181,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="60" spans="1:7" ht="17" x14ac:dyDescent="0.2">
+    <row r="60" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A60" s="3" t="s">
         <v>328</v>
       </c>
@@ -3198,7 +3204,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="61" spans="1:7" ht="17" x14ac:dyDescent="0.2">
+    <row r="61" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A61" s="3" t="s">
         <v>328</v>
       </c>
@@ -3221,7 +3227,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="62" spans="1:7" ht="17" x14ac:dyDescent="0.2">
+    <row r="62" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A62" s="3" t="s">
         <v>328</v>
       </c>
@@ -3244,7 +3250,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="63" spans="1:7" ht="17" x14ac:dyDescent="0.2">
+    <row r="63" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A63" s="3" t="s">
         <v>328</v>
       </c>
@@ -3267,7 +3273,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="64" spans="1:7" ht="17" x14ac:dyDescent="0.2">
+    <row r="64" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A64" s="3" t="s">
         <v>328</v>
       </c>
@@ -3290,7 +3296,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="65" spans="1:7" ht="17" x14ac:dyDescent="0.2">
+    <row r="65" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A65" s="3" t="s">
         <v>328</v>
       </c>
@@ -3313,7 +3319,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="66" spans="1:7" ht="17" x14ac:dyDescent="0.2">
+    <row r="66" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A66" s="3" t="s">
         <v>328</v>
       </c>
@@ -3336,7 +3342,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="67" spans="1:7" ht="17" x14ac:dyDescent="0.2">
+    <row r="67" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A67" s="3" t="s">
         <v>328</v>
       </c>
@@ -3359,7 +3365,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="68" spans="1:7" ht="17" x14ac:dyDescent="0.2">
+    <row r="68" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A68" s="3" t="s">
         <v>328</v>
       </c>
@@ -3382,7 +3388,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="69" spans="1:7" ht="17" x14ac:dyDescent="0.2">
+    <row r="69" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A69" s="3" t="s">
         <v>328</v>
       </c>
@@ -3405,7 +3411,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="70" spans="1:7" ht="17" x14ac:dyDescent="0.2">
+    <row r="70" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A70" s="3" t="s">
         <v>328</v>
       </c>
@@ -3428,7 +3434,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="71" spans="1:7" ht="17" x14ac:dyDescent="0.2">
+    <row r="71" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A71" s="3" t="s">
         <v>328</v>
       </c>
@@ -3451,7 +3457,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="72" spans="1:7" ht="17" x14ac:dyDescent="0.2">
+    <row r="72" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A72" s="3" t="s">
         <v>328</v>
       </c>
@@ -3474,7 +3480,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="73" spans="1:7" ht="17" x14ac:dyDescent="0.2">
+    <row r="73" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A73" s="3" t="s">
         <v>328</v>
       </c>
@@ -3497,7 +3503,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="74" spans="1:7" ht="17" x14ac:dyDescent="0.2">
+    <row r="74" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A74" s="3" t="s">
         <v>328</v>
       </c>
@@ -3520,7 +3526,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="75" spans="1:7" ht="17" x14ac:dyDescent="0.2">
+    <row r="75" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A75" s="3" t="s">
         <v>328</v>
       </c>
@@ -3543,7 +3549,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="76" spans="1:7" ht="17" x14ac:dyDescent="0.2">
+    <row r="76" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A76" s="3" t="s">
         <v>328</v>
       </c>
@@ -3566,7 +3572,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="77" spans="1:7" ht="17" x14ac:dyDescent="0.2">
+    <row r="77" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A77" s="3" t="s">
         <v>328</v>
       </c>
@@ -3589,7 +3595,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="78" spans="1:7" ht="17" x14ac:dyDescent="0.2">
+    <row r="78" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A78" s="3" t="s">
         <v>328</v>
       </c>
@@ -3612,7 +3618,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="79" spans="1:7" ht="17" x14ac:dyDescent="0.2">
+    <row r="79" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A79" s="3" t="s">
         <v>328</v>
       </c>
@@ -3635,7 +3641,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="80" spans="1:7" ht="17" x14ac:dyDescent="0.2">
+    <row r="80" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A80" s="3" t="s">
         <v>328</v>
       </c>
@@ -3658,7 +3664,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="81" spans="1:7" ht="17" x14ac:dyDescent="0.2">
+    <row r="81" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A81" s="3" t="s">
         <v>328</v>
       </c>
@@ -3681,7 +3687,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="82" spans="1:7" ht="17" x14ac:dyDescent="0.2">
+    <row r="82" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A82" s="3" t="s">
         <v>328</v>
       </c>
@@ -3704,7 +3710,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="83" spans="1:7" ht="17" x14ac:dyDescent="0.2">
+    <row r="83" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A83" s="3" t="s">
         <v>328</v>
       </c>
@@ -3727,7 +3733,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="84" spans="1:7" ht="17" x14ac:dyDescent="0.2">
+    <row r="84" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A84" s="3" t="s">
         <v>328</v>
       </c>
@@ -3750,7 +3756,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="85" spans="1:7" ht="17" x14ac:dyDescent="0.2">
+    <row r="85" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A85" s="3" t="s">
         <v>328</v>
       </c>
@@ -3773,7 +3779,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="86" spans="1:7" ht="17" x14ac:dyDescent="0.2">
+    <row r="86" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A86" s="3" t="s">
         <v>328</v>
       </c>
@@ -3796,7 +3802,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="87" spans="1:7" ht="17" x14ac:dyDescent="0.2">
+    <row r="87" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A87" s="3" t="s">
         <v>328</v>
       </c>
@@ -3819,7 +3825,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="88" spans="1:7" ht="17" x14ac:dyDescent="0.2">
+    <row r="88" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A88" s="3" t="s">
         <v>328</v>
       </c>
@@ -3842,7 +3848,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="89" spans="1:7" ht="17" x14ac:dyDescent="0.2">
+    <row r="89" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A89" s="3" t="s">
         <v>328</v>
       </c>
@@ -3865,7 +3871,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="90" spans="1:7" ht="17" x14ac:dyDescent="0.2">
+    <row r="90" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A90" s="3" t="s">
         <v>328</v>
       </c>
@@ -3888,7 +3894,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="91" spans="1:7" ht="17" x14ac:dyDescent="0.2">
+    <row r="91" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A91" s="3" t="s">
         <v>328</v>
       </c>
@@ -3911,7 +3917,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="92" spans="1:7" ht="17" x14ac:dyDescent="0.2">
+    <row r="92" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A92" s="3" t="s">
         <v>328</v>
       </c>
@@ -3934,7 +3940,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="93" spans="1:7" ht="17" x14ac:dyDescent="0.2">
+    <row r="93" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A93" s="3" t="s">
         <v>328</v>
       </c>
@@ -3957,7 +3963,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="94" spans="1:7" ht="17" x14ac:dyDescent="0.2">
+    <row r="94" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A94" s="3" t="s">
         <v>328</v>
       </c>
@@ -3980,7 +3986,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="95" spans="1:7" ht="17" x14ac:dyDescent="0.2">
+    <row r="95" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A95" s="3" t="s">
         <v>328</v>
       </c>
@@ -4003,7 +4009,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="96" spans="1:7" ht="17" x14ac:dyDescent="0.2">
+    <row r="96" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A96" s="3" t="s">
         <v>328</v>
       </c>
@@ -4026,7 +4032,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="97" spans="1:7" ht="17" x14ac:dyDescent="0.2">
+    <row r="97" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A97" s="3" t="s">
         <v>328</v>
       </c>
@@ -4049,7 +4055,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="98" spans="1:7" ht="17" x14ac:dyDescent="0.2">
+    <row r="98" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A98" s="3" t="s">
         <v>328</v>
       </c>
@@ -4072,7 +4078,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="99" spans="1:7" ht="17" x14ac:dyDescent="0.2">
+    <row r="99" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A99" s="3" t="s">
         <v>328</v>
       </c>
@@ -4095,7 +4101,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="100" spans="1:7" ht="17" x14ac:dyDescent="0.2">
+    <row r="100" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A100" s="3" t="s">
         <v>328</v>
       </c>
@@ -4118,7 +4124,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="101" spans="1:7" ht="17" x14ac:dyDescent="0.2">
+    <row r="101" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A101" s="3" t="s">
         <v>328</v>
       </c>
@@ -4141,7 +4147,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="102" spans="1:7" ht="17" x14ac:dyDescent="0.2">
+    <row r="102" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A102" s="3" t="s">
         <v>328</v>
       </c>
@@ -4164,7 +4170,7 @@
         <v>0.2</v>
       </c>
     </row>
-    <row r="103" spans="1:7" ht="17" x14ac:dyDescent="0.2">
+    <row r="103" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A103" s="3" t="s">
         <v>328</v>
       </c>
@@ -4187,7 +4193,7 @@
         <v>0.5</v>
       </c>
     </row>
-    <row r="104" spans="1:7" ht="17" x14ac:dyDescent="0.2">
+    <row r="104" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A104" s="3" t="s">
         <v>328</v>
       </c>
@@ -4210,7 +4216,7 @@
         <v>1.2</v>
       </c>
     </row>
-    <row r="105" spans="1:7" ht="17" x14ac:dyDescent="0.2">
+    <row r="105" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A105" s="3" t="s">
         <v>328</v>
       </c>
@@ -4233,7 +4239,7 @@
         <v>1.5</v>
       </c>
     </row>
-    <row r="106" spans="1:7" ht="17" x14ac:dyDescent="0.2">
+    <row r="106" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A106" s="3" t="s">
         <v>328</v>
       </c>
@@ -4256,7 +4262,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="107" spans="1:7" ht="17" x14ac:dyDescent="0.2">
+    <row r="107" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A107" s="3" t="s">
         <v>328</v>
       </c>
@@ -4279,7 +4285,7 @@
         <v>2.46</v>
       </c>
     </row>
-    <row r="108" spans="1:7" ht="17" x14ac:dyDescent="0.2">
+    <row r="108" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A108" s="3" t="s">
         <v>328</v>
       </c>
@@ -4302,7 +4308,7 @@
         <v>2.92</v>
       </c>
     </row>
-    <row r="109" spans="1:7" ht="17" x14ac:dyDescent="0.2">
+    <row r="109" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A109" s="3" t="s">
         <v>328</v>
       </c>
@@ -4325,7 +4331,7 @@
         <v>3.38</v>
       </c>
     </row>
-    <row r="110" spans="1:7" ht="17" x14ac:dyDescent="0.2">
+    <row r="110" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A110" s="3" t="s">
         <v>328</v>
       </c>
@@ -4348,7 +4354,7 @@
         <v>3.84</v>
       </c>
     </row>
-    <row r="111" spans="1:7" ht="17" x14ac:dyDescent="0.2">
+    <row r="111" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A111" s="3" t="s">
         <v>328</v>
       </c>
@@ -4371,7 +4377,7 @@
         <v>4.3</v>
       </c>
     </row>
-    <row r="112" spans="1:7" ht="17" x14ac:dyDescent="0.2">
+    <row r="112" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A112" s="3" t="s">
         <v>328</v>
       </c>
@@ -4394,7 +4400,7 @@
         <v>4.76</v>
       </c>
     </row>
-    <row r="113" spans="1:7" ht="17" x14ac:dyDescent="0.2">
+    <row r="113" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A113" s="3" t="s">
         <v>328</v>
       </c>
@@ -4417,7 +4423,7 @@
         <v>5.22</v>
       </c>
     </row>
-    <row r="114" spans="1:7" ht="17" x14ac:dyDescent="0.2">
+    <row r="114" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A114" s="3" t="s">
         <v>328</v>
       </c>
@@ -4440,7 +4446,7 @@
         <v>5.68</v>
       </c>
     </row>
-    <row r="115" spans="1:7" ht="17" x14ac:dyDescent="0.2">
+    <row r="115" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A115" s="3" t="s">
         <v>328</v>
       </c>
@@ -4463,7 +4469,7 @@
         <v>6.14</v>
       </c>
     </row>
-    <row r="116" spans="1:7" ht="17" x14ac:dyDescent="0.2">
+    <row r="116" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A116" s="3" t="s">
         <v>328</v>
       </c>
@@ -4486,7 +4492,7 @@
         <v>6.6</v>
       </c>
     </row>
-    <row r="117" spans="1:7" ht="17" x14ac:dyDescent="0.2">
+    <row r="117" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A117" s="3" t="s">
         <v>328</v>
       </c>
@@ -4509,7 +4515,7 @@
         <v>7.06</v>
       </c>
     </row>
-    <row r="118" spans="1:7" ht="17" x14ac:dyDescent="0.2">
+    <row r="118" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A118" s="3" t="s">
         <v>328</v>
       </c>
@@ -4532,7 +4538,7 @@
         <v>7.52</v>
       </c>
     </row>
-    <row r="119" spans="1:7" ht="17" x14ac:dyDescent="0.2">
+    <row r="119" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A119" s="3" t="s">
         <v>328</v>
       </c>
@@ -4555,7 +4561,7 @@
         <v>7.98</v>
       </c>
     </row>
-    <row r="120" spans="1:7" ht="17" x14ac:dyDescent="0.2">
+    <row r="120" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A120" s="3" t="s">
         <v>328</v>
       </c>
@@ -4578,7 +4584,7 @@
         <v>8.44</v>
       </c>
     </row>
-    <row r="121" spans="1:7" ht="17" x14ac:dyDescent="0.2">
+    <row r="121" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A121" s="3" t="s">
         <v>328</v>
       </c>
@@ -4601,7 +4607,7 @@
         <v>8.9</v>
       </c>
     </row>
-    <row r="122" spans="1:7" ht="17" x14ac:dyDescent="0.2">
+    <row r="122" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A122" s="3" t="s">
         <v>328</v>
       </c>
@@ -4624,7 +4630,7 @@
         <v>9.36</v>
       </c>
     </row>
-    <row r="123" spans="1:7" ht="17" x14ac:dyDescent="0.2">
+    <row r="123" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A123" s="3" t="s">
         <v>328</v>
       </c>
@@ -4647,7 +4653,7 @@
         <v>9.82</v>
       </c>
     </row>
-    <row r="124" spans="1:7" ht="17" x14ac:dyDescent="0.2">
+    <row r="124" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A124" s="3" t="s">
         <v>328</v>
       </c>
@@ -4670,7 +4676,7 @@
         <v>2.46</v>
       </c>
     </row>
-    <row r="125" spans="1:7" ht="17" x14ac:dyDescent="0.2">
+    <row r="125" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A125" s="3" t="s">
         <v>328</v>
       </c>
@@ -4693,7 +4699,7 @@
         <v>2.92</v>
       </c>
     </row>
-    <row r="126" spans="1:7" ht="17" x14ac:dyDescent="0.2">
+    <row r="126" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A126" s="3" t="s">
         <v>328</v>
       </c>
@@ -4716,7 +4722,7 @@
         <v>3.38</v>
       </c>
     </row>
-    <row r="127" spans="1:7" ht="17" x14ac:dyDescent="0.2">
+    <row r="127" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A127" s="3" t="s">
         <v>328</v>
       </c>
@@ -4739,7 +4745,7 @@
         <v>3.84</v>
       </c>
     </row>
-    <row r="128" spans="1:7" ht="17" x14ac:dyDescent="0.2">
+    <row r="128" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A128" s="3" t="s">
         <v>328</v>
       </c>
@@ -4762,7 +4768,7 @@
         <v>4.3</v>
       </c>
     </row>
-    <row r="129" spans="1:7" ht="17" x14ac:dyDescent="0.2">
+    <row r="129" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A129" s="3" t="s">
         <v>328</v>
       </c>
@@ -4785,7 +4791,7 @@
         <v>4.76</v>
       </c>
     </row>
-    <row r="130" spans="1:7" ht="17" x14ac:dyDescent="0.2">
+    <row r="130" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A130" s="3" t="s">
         <v>328</v>
       </c>
@@ -4808,7 +4814,7 @@
         <v>5.22</v>
       </c>
     </row>
-    <row r="131" spans="1:7" ht="17" x14ac:dyDescent="0.2">
+    <row r="131" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A131" s="3" t="s">
         <v>328</v>
       </c>
@@ -4831,7 +4837,7 @@
         <v>5.68</v>
       </c>
     </row>
-    <row r="132" spans="1:7" ht="17" x14ac:dyDescent="0.2">
+    <row r="132" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A132" s="3" t="s">
         <v>328</v>
       </c>
@@ -4854,7 +4860,7 @@
         <v>6.14</v>
       </c>
     </row>
-    <row r="133" spans="1:7" ht="17" x14ac:dyDescent="0.2">
+    <row r="133" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A133" s="3" t="s">
         <v>328</v>
       </c>
@@ -4877,7 +4883,7 @@
         <v>6.6</v>
       </c>
     </row>
-    <row r="134" spans="1:7" ht="17" x14ac:dyDescent="0.2">
+    <row r="134" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A134" s="3" t="s">
         <v>328</v>
       </c>
@@ -4900,7 +4906,7 @@
         <v>7.06</v>
       </c>
     </row>
-    <row r="135" spans="1:7" ht="17" x14ac:dyDescent="0.2">
+    <row r="135" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A135" s="3" t="s">
         <v>328</v>
       </c>
@@ -4923,7 +4929,7 @@
         <v>7.52</v>
       </c>
     </row>
-    <row r="136" spans="1:7" ht="17" x14ac:dyDescent="0.2">
+    <row r="136" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A136" s="3" t="s">
         <v>328</v>
       </c>
@@ -4946,7 +4952,7 @@
         <v>7.98</v>
       </c>
     </row>
-    <row r="137" spans="1:7" ht="17" x14ac:dyDescent="0.2">
+    <row r="137" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A137" s="3" t="s">
         <v>328</v>
       </c>
@@ -4969,7 +4975,7 @@
         <v>8.44</v>
       </c>
     </row>
-    <row r="138" spans="1:7" ht="17" x14ac:dyDescent="0.2">
+    <row r="138" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A138" s="3" t="s">
         <v>328</v>
       </c>
@@ -4992,7 +4998,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="139" spans="1:7" ht="17" x14ac:dyDescent="0.2">
+    <row r="139" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A139" s="3" t="s">
         <v>328</v>
       </c>
@@ -5015,7 +5021,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="140" spans="1:7" ht="17" x14ac:dyDescent="0.2">
+    <row r="140" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A140" s="3" t="s">
         <v>328</v>
       </c>
@@ -5038,7 +5044,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="141" spans="1:7" ht="17" x14ac:dyDescent="0.2">
+    <row r="141" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A141" s="3" t="s">
         <v>328</v>
       </c>
@@ -5061,7 +5067,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="142" spans="1:7" ht="17" x14ac:dyDescent="0.2">
+    <row r="142" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A142" s="3" t="s">
         <v>328</v>
       </c>
@@ -5084,7 +5090,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="143" spans="1:7" ht="17" x14ac:dyDescent="0.2">
+    <row r="143" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A143" s="3" t="s">
         <v>328</v>
       </c>
@@ -5107,7 +5113,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="144" spans="1:7" ht="17" x14ac:dyDescent="0.2">
+    <row r="144" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A144" s="3" t="s">
         <v>328</v>
       </c>
@@ -5130,7 +5136,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="145" spans="1:7" ht="17" x14ac:dyDescent="0.2">
+    <row r="145" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A145" s="3" t="s">
         <v>328</v>
       </c>
@@ -5153,7 +5159,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="146" spans="1:7" ht="17" x14ac:dyDescent="0.2">
+    <row r="146" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A146" s="3" t="s">
         <v>328</v>
       </c>
@@ -5176,7 +5182,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="147" spans="1:7" ht="17" x14ac:dyDescent="0.2">
+    <row r="147" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A147" s="3" t="s">
         <v>328</v>
       </c>
@@ -5199,7 +5205,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="148" spans="1:7" ht="17" x14ac:dyDescent="0.2">
+    <row r="148" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A148" s="3" t="s">
         <v>328</v>
       </c>
@@ -5222,7 +5228,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="149" spans="1:7" ht="17" x14ac:dyDescent="0.2">
+    <row r="149" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A149" s="3" t="s">
         <v>328</v>
       </c>
@@ -5245,7 +5251,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="150" spans="1:7" ht="17" x14ac:dyDescent="0.2">
+    <row r="150" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A150" s="3" t="s">
         <v>328</v>
       </c>
@@ -5268,7 +5274,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="151" spans="1:7" ht="17" x14ac:dyDescent="0.2">
+    <row r="151" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A151" s="3" t="s">
         <v>328</v>
       </c>
@@ -5291,7 +5297,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="152" spans="1:7" ht="17" x14ac:dyDescent="0.2">
+    <row r="152" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A152" s="3" t="s">
         <v>328</v>
       </c>
@@ -5314,7 +5320,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="153" spans="1:7" ht="17" x14ac:dyDescent="0.2">
+    <row r="153" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A153" s="3" t="s">
         <v>328</v>
       </c>
@@ -5337,7 +5343,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="154" spans="1:7" ht="17" x14ac:dyDescent="0.2">
+    <row r="154" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A154" s="3" t="s">
         <v>328</v>
       </c>
@@ -5360,7 +5366,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="155" spans="1:7" ht="17" x14ac:dyDescent="0.2">
+    <row r="155" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A155" s="3" t="s">
         <v>328</v>
       </c>
@@ -5383,7 +5389,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="156" spans="1:7" ht="17" x14ac:dyDescent="0.2">
+    <row r="156" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A156" s="3" t="s">
         <v>328</v>
       </c>
@@ -5406,7 +5412,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="157" spans="1:7" ht="17" x14ac:dyDescent="0.2">
+    <row r="157" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A157" s="3" t="s">
         <v>328</v>
       </c>
@@ -5429,7 +5435,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="158" spans="1:7" ht="17" x14ac:dyDescent="0.2">
+    <row r="158" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A158" s="3" t="s">
         <v>328</v>
       </c>
@@ -5452,7 +5458,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="159" spans="1:7" ht="17" x14ac:dyDescent="0.2">
+    <row r="159" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A159" s="3" t="s">
         <v>328</v>
       </c>
@@ -5475,7 +5481,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="160" spans="1:7" ht="17" x14ac:dyDescent="0.2">
+    <row r="160" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A160" s="3" t="s">
         <v>328</v>
       </c>
@@ -5498,7 +5504,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="161" spans="1:7" ht="17" x14ac:dyDescent="0.2">
+    <row r="161" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A161" s="3" t="s">
         <v>328</v>
       </c>
@@ -5521,7 +5527,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="162" spans="1:7" ht="17" x14ac:dyDescent="0.2">
+    <row r="162" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A162" s="3" t="s">
         <v>328</v>
       </c>
@@ -5547,6 +5553,7 @@
   </sheetData>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
   <ignoredErrors>
     <ignoredError sqref="G1 A1:D1" numberStoredAsText="1"/>
   </ignoredErrors>

</xml_diff>